<commit_message>
All impacts in progbook except latent
Using Optima TB impact factors as maximum values for Atomica impacts, all Gauteng impacts have been transcribed, except for the tricky latent case.
It is yet to be seen if extra cells must be filled out or cause problems during progbook parsing.
</commit_message>
<xml_diff>
--- a/tests/databooks/progbook_tb.xlsx
+++ b/tests/databooks/progbook_tb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2594CB-1750-4115-84E9-1B2D581029E8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE46A450-7302-4FE3-A019-CDFDBC469CBD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Program data" sheetId="2" r:id="rId2"/>
     <sheet name="Program effects" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017" calcMode="manual"/>
+  <calcPr calcId="179017" calcMode="manual" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1057,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU33"/>
   <sheetViews>
-    <sheetView topLeftCell="AA7" workbookViewId="0">
-      <selection activeCell="AI22" sqref="AI22:AS23"/>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2754,7 +2754,9 @@
       <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
       <c r="AB24" s="4"/>
-      <c r="AC24" s="4"/>
+      <c r="AC24" s="4">
+        <v>1</v>
+      </c>
       <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
       <c r="AF24" s="4"/>
@@ -2764,7 +2766,9 @@
       <c r="AJ24" s="4"/>
       <c r="AK24" s="4"/>
       <c r="AL24" s="4"/>
-      <c r="AM24" s="4"/>
+      <c r="AM24" s="4">
+        <v>1</v>
+      </c>
       <c r="AN24" s="4"/>
       <c r="AO24" s="4"/>
       <c r="AP24" s="4"/>
@@ -2811,7 +2815,9 @@
       <c r="AC25" s="4"/>
       <c r="AD25" s="4"/>
       <c r="AE25" s="4"/>
-      <c r="AF25" s="4"/>
+      <c r="AF25" s="4">
+        <v>1</v>
+      </c>
       <c r="AG25" s="4"/>
       <c r="AH25" s="4"/>
       <c r="AI25" s="4"/>
@@ -2821,7 +2827,9 @@
       <c r="AM25" s="4"/>
       <c r="AN25" s="4"/>
       <c r="AO25" s="4"/>
-      <c r="AP25" s="4"/>
+      <c r="AP25" s="4">
+        <v>1</v>
+      </c>
       <c r="AQ25" s="4"/>
       <c r="AR25" s="4"/>
       <c r="AS25" s="4"/>
@@ -2868,7 +2876,9 @@
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
       <c r="AH26" s="4"/>
-      <c r="AI26" s="4"/>
+      <c r="AI26" s="4">
+        <v>1</v>
+      </c>
       <c r="AJ26" s="4"/>
       <c r="AK26" s="4"/>
       <c r="AL26" s="4"/>
@@ -2878,7 +2888,9 @@
       <c r="AP26" s="4"/>
       <c r="AQ26" s="4"/>
       <c r="AR26" s="4"/>
-      <c r="AS26" s="4"/>
+      <c r="AS26" s="4">
+        <v>1</v>
+      </c>
       <c r="AT26" s="4"/>
       <c r="AU26" s="4"/>
     </row>
@@ -2916,7 +2928,9 @@
       <c r="Z27" s="4"/>
       <c r="AA27" s="4"/>
       <c r="AB27" s="4"/>
-      <c r="AC27" s="4"/>
+      <c r="AC27" s="4">
+        <v>1</v>
+      </c>
       <c r="AD27" s="4"/>
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
@@ -2926,7 +2940,9 @@
       <c r="AJ27" s="4"/>
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
-      <c r="AM27" s="4"/>
+      <c r="AM27" s="4">
+        <v>1</v>
+      </c>
       <c r="AN27" s="4"/>
       <c r="AO27" s="4"/>
       <c r="AP27" s="4"/>
@@ -2973,7 +2989,9 @@
       <c r="AC28" s="4"/>
       <c r="AD28" s="4"/>
       <c r="AE28" s="4"/>
-      <c r="AF28" s="4"/>
+      <c r="AF28" s="4">
+        <v>1</v>
+      </c>
       <c r="AG28" s="4"/>
       <c r="AH28" s="4"/>
       <c r="AI28" s="4"/>
@@ -2983,7 +3001,9 @@
       <c r="AM28" s="4"/>
       <c r="AN28" s="4"/>
       <c r="AO28" s="4"/>
-      <c r="AP28" s="4"/>
+      <c r="AP28" s="4">
+        <v>1</v>
+      </c>
       <c r="AQ28" s="4"/>
       <c r="AR28" s="4"/>
       <c r="AS28" s="4"/>
@@ -3030,7 +3050,9 @@
       <c r="AF29" s="4"/>
       <c r="AG29" s="4"/>
       <c r="AH29" s="4"/>
-      <c r="AI29" s="4"/>
+      <c r="AI29" s="4">
+        <v>1</v>
+      </c>
       <c r="AJ29" s="4"/>
       <c r="AK29" s="4"/>
       <c r="AL29" s="4"/>
@@ -3040,7 +3062,9 @@
       <c r="AP29" s="4"/>
       <c r="AQ29" s="4"/>
       <c r="AR29" s="4"/>
-      <c r="AS29" s="4"/>
+      <c r="AS29" s="4">
+        <v>1</v>
+      </c>
       <c r="AT29" s="4"/>
       <c r="AU29" s="4"/>
     </row>
@@ -6647,10 +6671,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AK1037"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="G1017" sqref="G1017"/>
+      <selection pane="bottomLeft" activeCell="T1002" sqref="T1002:AG1037"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14485,7 +14509,9 @@
       <c r="K188" s="4"/>
       <c r="L188" s="4"/>
       <c r="M188" s="4"/>
-      <c r="N188" s="4"/>
+      <c r="N188" s="4">
+        <v>1</v>
+      </c>
       <c r="O188" s="4"/>
       <c r="P188" s="4"/>
       <c r="Q188" s="4"/>
@@ -14611,7 +14637,9 @@
       <c r="K191" s="4"/>
       <c r="L191" s="4"/>
       <c r="M191" s="4"/>
-      <c r="N191" s="4"/>
+      <c r="N191" s="4">
+        <v>1</v>
+      </c>
       <c r="O191" s="4"/>
       <c r="P191" s="4"/>
       <c r="Q191" s="4"/>
@@ -14737,7 +14765,9 @@
       <c r="K194" s="4"/>
       <c r="L194" s="4"/>
       <c r="M194" s="4"/>
-      <c r="N194" s="4"/>
+      <c r="N194" s="4">
+        <v>1</v>
+      </c>
       <c r="O194" s="4"/>
       <c r="P194" s="4"/>
       <c r="Q194" s="4"/>
@@ -14863,7 +14893,9 @@
       <c r="K197" s="4"/>
       <c r="L197" s="4"/>
       <c r="M197" s="4"/>
-      <c r="N197" s="4"/>
+      <c r="N197" s="4">
+        <v>1</v>
+      </c>
       <c r="O197" s="4"/>
       <c r="P197" s="4"/>
       <c r="Q197" s="4"/>
@@ -14997,7 +15029,9 @@
       <c r="S200" s="4"/>
       <c r="T200" s="4"/>
       <c r="U200" s="4"/>
-      <c r="V200" s="4"/>
+      <c r="V200" s="4">
+        <v>1</v>
+      </c>
       <c r="W200" s="4"/>
       <c r="X200" s="4"/>
       <c r="Y200" s="4"/>
@@ -15123,7 +15157,9 @@
       <c r="S203" s="4"/>
       <c r="T203" s="4"/>
       <c r="U203" s="4"/>
-      <c r="V203" s="4"/>
+      <c r="V203" s="4">
+        <v>1</v>
+      </c>
       <c r="W203" s="4"/>
       <c r="X203" s="4"/>
       <c r="Y203" s="4"/>
@@ -15241,7 +15277,9 @@
       <c r="K206" s="4"/>
       <c r="L206" s="4"/>
       <c r="M206" s="4"/>
-      <c r="N206" s="4"/>
+      <c r="N206" s="4">
+        <v>1</v>
+      </c>
       <c r="O206" s="4"/>
       <c r="P206" s="4"/>
       <c r="Q206" s="4"/>
@@ -15255,7 +15293,9 @@
       <c r="Y206" s="4"/>
       <c r="Z206" s="4"/>
       <c r="AA206" s="4"/>
-      <c r="AB206" s="4"/>
+      <c r="AB206" s="4">
+        <v>1</v>
+      </c>
       <c r="AC206" s="4"/>
       <c r="AD206" s="4"/>
       <c r="AE206" s="4"/>
@@ -15375,13 +15415,17 @@
       <c r="S209" s="4"/>
       <c r="T209" s="4"/>
       <c r="U209" s="4"/>
-      <c r="V209" s="4"/>
+      <c r="V209" s="4">
+        <v>1</v>
+      </c>
       <c r="W209" s="4"/>
       <c r="X209" s="4"/>
       <c r="Y209" s="4"/>
       <c r="Z209" s="4"/>
       <c r="AA209" s="4"/>
-      <c r="AB209" s="4"/>
+      <c r="AB209" s="4">
+        <v>1</v>
+      </c>
       <c r="AC209" s="4"/>
       <c r="AD209" s="4"/>
       <c r="AE209" s="4"/>
@@ -15745,7 +15789,9 @@
       <c r="K218" s="4"/>
       <c r="L218" s="4"/>
       <c r="M218" s="4"/>
-      <c r="N218" s="4"/>
+      <c r="N218" s="4">
+        <v>1</v>
+      </c>
       <c r="O218" s="4"/>
       <c r="P218" s="4"/>
       <c r="Q218" s="4"/>
@@ -15762,7 +15808,9 @@
       <c r="AB218" s="4"/>
       <c r="AC218" s="4"/>
       <c r="AD218" s="4"/>
-      <c r="AE218" s="4"/>
+      <c r="AE218" s="4">
+        <v>1</v>
+      </c>
       <c r="AF218" s="4"/>
       <c r="AG218" s="4"/>
       <c r="AH218" s="4"/>
@@ -15879,7 +15927,9 @@
       <c r="S221" s="4"/>
       <c r="T221" s="4"/>
       <c r="U221" s="4"/>
-      <c r="V221" s="4"/>
+      <c r="V221" s="4">
+        <v>1</v>
+      </c>
       <c r="W221" s="4"/>
       <c r="X221" s="4"/>
       <c r="Y221" s="4"/>
@@ -15888,7 +15938,9 @@
       <c r="AB221" s="4"/>
       <c r="AC221" s="4"/>
       <c r="AD221" s="4"/>
-      <c r="AE221" s="4"/>
+      <c r="AE221" s="4">
+        <v>1</v>
+      </c>
       <c r="AF221" s="4"/>
       <c r="AG221" s="4"/>
       <c r="AH221" s="4"/>
@@ -15997,7 +16049,9 @@
       <c r="K225" s="4"/>
       <c r="L225" s="4"/>
       <c r="M225" s="4"/>
-      <c r="N225" s="4"/>
+      <c r="N225" s="4">
+        <v>7.4999999999999956E-2</v>
+      </c>
       <c r="O225" s="4"/>
       <c r="P225" s="4"/>
       <c r="Q225" s="4"/>
@@ -16123,7 +16177,9 @@
       <c r="K228" s="4"/>
       <c r="L228" s="4"/>
       <c r="M228" s="4"/>
-      <c r="N228" s="4"/>
+      <c r="N228" s="4">
+        <v>7.4999999999999956E-2</v>
+      </c>
       <c r="O228" s="4"/>
       <c r="P228" s="4"/>
       <c r="Q228" s="4"/>
@@ -16249,7 +16305,9 @@
       <c r="K231" s="4"/>
       <c r="L231" s="4"/>
       <c r="M231" s="4"/>
-      <c r="N231" s="4"/>
+      <c r="N231" s="4">
+        <v>6.2E-2</v>
+      </c>
       <c r="O231" s="4"/>
       <c r="P231" s="4"/>
       <c r="Q231" s="4"/>
@@ -16375,7 +16433,9 @@
       <c r="K234" s="4"/>
       <c r="L234" s="4"/>
       <c r="M234" s="4"/>
-      <c r="N234" s="4"/>
+      <c r="N234" s="4">
+        <v>6.2E-2</v>
+      </c>
       <c r="O234" s="4"/>
       <c r="P234" s="4"/>
       <c r="Q234" s="4"/>
@@ -16509,7 +16569,9 @@
       <c r="S237" s="4"/>
       <c r="T237" s="4"/>
       <c r="U237" s="4"/>
-      <c r="V237" s="4"/>
+      <c r="V237" s="4">
+        <v>7.4999999999999956E-2</v>
+      </c>
       <c r="W237" s="4"/>
       <c r="X237" s="4"/>
       <c r="Y237" s="4"/>
@@ -16635,7 +16697,9 @@
       <c r="S240" s="4"/>
       <c r="T240" s="4"/>
       <c r="U240" s="4"/>
-      <c r="V240" s="4"/>
+      <c r="V240" s="4">
+        <v>7.4999999999999956E-2</v>
+      </c>
       <c r="W240" s="4"/>
       <c r="X240" s="4"/>
       <c r="Y240" s="4"/>
@@ -16753,7 +16817,9 @@
       <c r="K243" s="4"/>
       <c r="L243" s="4"/>
       <c r="M243" s="4"/>
-      <c r="N243" s="4"/>
+      <c r="N243" s="4">
+        <v>6.2E-2</v>
+      </c>
       <c r="O243" s="4"/>
       <c r="P243" s="4"/>
       <c r="Q243" s="4"/>
@@ -16767,7 +16833,9 @@
       <c r="Y243" s="4"/>
       <c r="Z243" s="4"/>
       <c r="AA243" s="4"/>
-      <c r="AB243" s="4"/>
+      <c r="AB243" s="4">
+        <v>0.04</v>
+      </c>
       <c r="AC243" s="4"/>
       <c r="AD243" s="4"/>
       <c r="AE243" s="4"/>
@@ -16887,13 +16955,17 @@
       <c r="S246" s="4"/>
       <c r="T246" s="4"/>
       <c r="U246" s="4"/>
-      <c r="V246" s="4"/>
+      <c r="V246" s="4">
+        <v>7.4999999999999956E-2</v>
+      </c>
       <c r="W246" s="4"/>
       <c r="X246" s="4"/>
       <c r="Y246" s="4"/>
       <c r="Z246" s="4"/>
       <c r="AA246" s="4"/>
-      <c r="AB246" s="4"/>
+      <c r="AB246" s="4">
+        <v>0.04</v>
+      </c>
       <c r="AC246" s="4"/>
       <c r="AD246" s="4"/>
       <c r="AE246" s="4"/>
@@ -17257,7 +17329,9 @@
       <c r="K255" s="4"/>
       <c r="L255" s="4"/>
       <c r="M255" s="4"/>
-      <c r="N255" s="4"/>
+      <c r="N255" s="4">
+        <v>6.2E-2</v>
+      </c>
       <c r="O255" s="4"/>
       <c r="P255" s="4"/>
       <c r="Q255" s="4"/>
@@ -17274,7 +17348,9 @@
       <c r="AB255" s="4"/>
       <c r="AC255" s="4"/>
       <c r="AD255" s="4"/>
-      <c r="AE255" s="4"/>
+      <c r="AE255" s="4">
+        <v>1</v>
+      </c>
       <c r="AF255" s="4"/>
       <c r="AG255" s="4"/>
       <c r="AH255" s="4"/>
@@ -17391,7 +17467,9 @@
       <c r="S258" s="4"/>
       <c r="T258" s="4"/>
       <c r="U258" s="4"/>
-      <c r="V258" s="4"/>
+      <c r="V258" s="4">
+        <v>7.4999999999999956E-2</v>
+      </c>
       <c r="W258" s="4"/>
       <c r="X258" s="4"/>
       <c r="Y258" s="4"/>
@@ -17400,7 +17478,9 @@
       <c r="AB258" s="4"/>
       <c r="AC258" s="4"/>
       <c r="AD258" s="4"/>
-      <c r="AE258" s="4"/>
+      <c r="AE258" s="4">
+        <v>1</v>
+      </c>
       <c r="AF258" s="4"/>
       <c r="AG258" s="4"/>
       <c r="AH258" s="4"/>
@@ -17509,7 +17589,9 @@
       <c r="K262" s="4"/>
       <c r="L262" s="4"/>
       <c r="M262" s="4"/>
-      <c r="N262" s="4"/>
+      <c r="N262" s="4">
+        <v>0.95673599999999992</v>
+      </c>
       <c r="O262" s="4"/>
       <c r="P262" s="4"/>
       <c r="Q262" s="4"/>
@@ -17635,7 +17717,9 @@
       <c r="K265" s="4"/>
       <c r="L265" s="4"/>
       <c r="M265" s="4"/>
-      <c r="N265" s="4"/>
+      <c r="N265" s="4">
+        <v>0.95673599999999992</v>
+      </c>
       <c r="O265" s="4"/>
       <c r="P265" s="4"/>
       <c r="Q265" s="4"/>
@@ -17761,7 +17845,9 @@
       <c r="K268" s="4"/>
       <c r="L268" s="4"/>
       <c r="M268" s="4"/>
-      <c r="N268" s="4"/>
+      <c r="N268" s="4">
+        <v>0.95673599999999992</v>
+      </c>
       <c r="O268" s="4"/>
       <c r="P268" s="4"/>
       <c r="Q268" s="4"/>
@@ -17887,7 +17973,9 @@
       <c r="K271" s="4"/>
       <c r="L271" s="4"/>
       <c r="M271" s="4"/>
-      <c r="N271" s="4"/>
+      <c r="N271" s="4">
+        <v>0.95673599999999992</v>
+      </c>
       <c r="O271" s="4"/>
       <c r="P271" s="4"/>
       <c r="Q271" s="4"/>
@@ -18021,7 +18109,9 @@
       <c r="S274" s="4"/>
       <c r="T274" s="4"/>
       <c r="U274" s="4"/>
-      <c r="V274" s="4"/>
+      <c r="V274" s="4">
+        <v>0.95247599999999999</v>
+      </c>
       <c r="W274" s="4"/>
       <c r="X274" s="4"/>
       <c r="Y274" s="4"/>
@@ -18147,7 +18237,9 @@
       <c r="S277" s="4"/>
       <c r="T277" s="4"/>
       <c r="U277" s="4"/>
-      <c r="V277" s="4"/>
+      <c r="V277" s="4">
+        <v>0.95247599999999999</v>
+      </c>
       <c r="W277" s="4"/>
       <c r="X277" s="4"/>
       <c r="Y277" s="4"/>
@@ -18265,7 +18357,9 @@
       <c r="K280" s="4"/>
       <c r="L280" s="4"/>
       <c r="M280" s="4"/>
-      <c r="N280" s="4"/>
+      <c r="N280" s="4">
+        <v>0.95673599999999992</v>
+      </c>
       <c r="O280" s="4"/>
       <c r="P280" s="4"/>
       <c r="Q280" s="4"/>
@@ -18279,7 +18373,9 @@
       <c r="Y280" s="4"/>
       <c r="Z280" s="4"/>
       <c r="AA280" s="4"/>
-      <c r="AB280" s="4"/>
+      <c r="AB280" s="4">
+        <v>0.99839999999999995</v>
+      </c>
       <c r="AC280" s="4"/>
       <c r="AD280" s="4"/>
       <c r="AE280" s="4"/>
@@ -18399,13 +18495,17 @@
       <c r="S283" s="4"/>
       <c r="T283" s="4"/>
       <c r="U283" s="4"/>
-      <c r="V283" s="4"/>
+      <c r="V283" s="4">
+        <v>0.95247599999999999</v>
+      </c>
       <c r="W283" s="4"/>
       <c r="X283" s="4"/>
       <c r="Y283" s="4"/>
       <c r="Z283" s="4"/>
       <c r="AA283" s="4"/>
-      <c r="AB283" s="4"/>
+      <c r="AB283" s="4">
+        <v>0.99839999999999995</v>
+      </c>
       <c r="AC283" s="4"/>
       <c r="AD283" s="4"/>
       <c r="AE283" s="4"/>
@@ -18769,7 +18869,9 @@
       <c r="K292" s="4"/>
       <c r="L292" s="4"/>
       <c r="M292" s="4"/>
-      <c r="N292" s="4"/>
+      <c r="N292" s="4">
+        <v>0.95673599999999992</v>
+      </c>
       <c r="O292" s="4"/>
       <c r="P292" s="4"/>
       <c r="Q292" s="4"/>
@@ -18786,7 +18888,9 @@
       <c r="AB292" s="4"/>
       <c r="AC292" s="4"/>
       <c r="AD292" s="4"/>
-      <c r="AE292" s="4"/>
+      <c r="AE292" s="4">
+        <v>0</v>
+      </c>
       <c r="AF292" s="4"/>
       <c r="AG292" s="4"/>
       <c r="AH292" s="4"/>
@@ -18903,7 +19007,9 @@
       <c r="S295" s="4"/>
       <c r="T295" s="4"/>
       <c r="U295" s="4"/>
-      <c r="V295" s="4"/>
+      <c r="V295" s="4">
+        <v>0.95247599999999999</v>
+      </c>
       <c r="W295" s="4"/>
       <c r="X295" s="4"/>
       <c r="Y295" s="4"/>
@@ -18912,7 +19018,9 @@
       <c r="AB295" s="4"/>
       <c r="AC295" s="4"/>
       <c r="AD295" s="4"/>
-      <c r="AE295" s="4"/>
+      <c r="AE295" s="4">
+        <v>0</v>
+      </c>
       <c r="AF295" s="4"/>
       <c r="AG295" s="4"/>
       <c r="AH295" s="4"/>
@@ -20616,11 +20724,21 @@
       <c r="L336" s="4"/>
       <c r="M336" s="4"/>
       <c r="N336" s="4"/>
-      <c r="O336" s="4"/>
-      <c r="P336" s="4"/>
-      <c r="Q336" s="4"/>
-      <c r="R336" s="4"/>
-      <c r="S336" s="4"/>
+      <c r="O336" s="4">
+        <v>1</v>
+      </c>
+      <c r="P336" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q336" s="4">
+        <v>1</v>
+      </c>
+      <c r="R336" s="4">
+        <v>1</v>
+      </c>
+      <c r="S336" s="4">
+        <v>1</v>
+      </c>
       <c r="T336" s="4"/>
       <c r="U336" s="4"/>
       <c r="V336" s="4"/>
@@ -20742,11 +20860,21 @@
       <c r="L339" s="4"/>
       <c r="M339" s="4"/>
       <c r="N339" s="4"/>
-      <c r="O339" s="4"/>
-      <c r="P339" s="4"/>
-      <c r="Q339" s="4"/>
-      <c r="R339" s="4"/>
-      <c r="S339" s="4"/>
+      <c r="O339" s="4">
+        <v>1</v>
+      </c>
+      <c r="P339" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q339" s="4">
+        <v>1</v>
+      </c>
+      <c r="R339" s="4">
+        <v>1</v>
+      </c>
+      <c r="S339" s="4">
+        <v>1</v>
+      </c>
       <c r="T339" s="4"/>
       <c r="U339" s="4"/>
       <c r="V339" s="4"/>
@@ -20868,11 +20996,21 @@
       <c r="L342" s="4"/>
       <c r="M342" s="4"/>
       <c r="N342" s="4"/>
-      <c r="O342" s="4"/>
-      <c r="P342" s="4"/>
-      <c r="Q342" s="4"/>
-      <c r="R342" s="4"/>
-      <c r="S342" s="4"/>
+      <c r="O342" s="4">
+        <v>1</v>
+      </c>
+      <c r="P342" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q342" s="4">
+        <v>1</v>
+      </c>
+      <c r="R342" s="4">
+        <v>1</v>
+      </c>
+      <c r="S342" s="4">
+        <v>1</v>
+      </c>
       <c r="T342" s="4"/>
       <c r="U342" s="4"/>
       <c r="V342" s="4"/>
@@ -20994,11 +21132,21 @@
       <c r="L345" s="4"/>
       <c r="M345" s="4"/>
       <c r="N345" s="4"/>
-      <c r="O345" s="4"/>
-      <c r="P345" s="4"/>
-      <c r="Q345" s="4"/>
-      <c r="R345" s="4"/>
-      <c r="S345" s="4"/>
+      <c r="O345" s="4">
+        <v>1</v>
+      </c>
+      <c r="P345" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q345" s="4">
+        <v>1</v>
+      </c>
+      <c r="R345" s="4">
+        <v>1</v>
+      </c>
+      <c r="S345" s="4">
+        <v>1</v>
+      </c>
       <c r="T345" s="4"/>
       <c r="U345" s="4"/>
       <c r="V345" s="4"/>
@@ -21128,9 +21276,15 @@
       <c r="T348" s="4"/>
       <c r="U348" s="4"/>
       <c r="V348" s="4"/>
-      <c r="W348" s="4"/>
-      <c r="X348" s="4"/>
-      <c r="Y348" s="4"/>
+      <c r="W348" s="4">
+        <v>1</v>
+      </c>
+      <c r="X348" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y348" s="4">
+        <v>1</v>
+      </c>
       <c r="Z348" s="4"/>
       <c r="AA348" s="4"/>
       <c r="AB348" s="4"/>
@@ -21254,9 +21408,15 @@
       <c r="T351" s="4"/>
       <c r="U351" s="4"/>
       <c r="V351" s="4"/>
-      <c r="W351" s="4"/>
-      <c r="X351" s="4"/>
-      <c r="Y351" s="4"/>
+      <c r="W351" s="4">
+        <v>1</v>
+      </c>
+      <c r="X351" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y351" s="4">
+        <v>1</v>
+      </c>
       <c r="Z351" s="4"/>
       <c r="AA351" s="4"/>
       <c r="AB351" s="4"/>
@@ -21372,11 +21532,21 @@
       <c r="L354" s="4"/>
       <c r="M354" s="4"/>
       <c r="N354" s="4"/>
-      <c r="O354" s="4"/>
-      <c r="P354" s="4"/>
-      <c r="Q354" s="4"/>
-      <c r="R354" s="4"/>
-      <c r="S354" s="4"/>
+      <c r="O354" s="4">
+        <v>1</v>
+      </c>
+      <c r="P354" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q354" s="4">
+        <v>1</v>
+      </c>
+      <c r="R354" s="4">
+        <v>1</v>
+      </c>
+      <c r="S354" s="4">
+        <v>1</v>
+      </c>
       <c r="T354" s="4"/>
       <c r="U354" s="4"/>
       <c r="V354" s="4"/>
@@ -21386,7 +21556,9 @@
       <c r="Z354" s="4"/>
       <c r="AA354" s="4"/>
       <c r="AB354" s="4"/>
-      <c r="AC354" s="4"/>
+      <c r="AC354" s="4">
+        <v>1</v>
+      </c>
       <c r="AD354" s="4"/>
       <c r="AE354" s="4"/>
       <c r="AF354" s="4"/>
@@ -21506,13 +21678,21 @@
       <c r="T357" s="4"/>
       <c r="U357" s="4"/>
       <c r="V357" s="4"/>
-      <c r="W357" s="4"/>
-      <c r="X357" s="4"/>
-      <c r="Y357" s="4"/>
+      <c r="W357" s="4">
+        <v>1</v>
+      </c>
+      <c r="X357" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y357" s="4">
+        <v>1</v>
+      </c>
       <c r="Z357" s="4"/>
       <c r="AA357" s="4"/>
       <c r="AB357" s="4"/>
-      <c r="AC357" s="4"/>
+      <c r="AC357" s="4">
+        <v>1</v>
+      </c>
       <c r="AD357" s="4"/>
       <c r="AE357" s="4"/>
       <c r="AF357" s="4"/>
@@ -21876,11 +22056,21 @@
       <c r="L366" s="4"/>
       <c r="M366" s="4"/>
       <c r="N366" s="4"/>
-      <c r="O366" s="4"/>
-      <c r="P366" s="4"/>
-      <c r="Q366" s="4"/>
-      <c r="R366" s="4"/>
-      <c r="S366" s="4"/>
+      <c r="O366" s="4">
+        <v>1</v>
+      </c>
+      <c r="P366" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q366" s="4">
+        <v>1</v>
+      </c>
+      <c r="R366" s="4">
+        <v>1</v>
+      </c>
+      <c r="S366" s="4">
+        <v>1</v>
+      </c>
       <c r="T366" s="4"/>
       <c r="U366" s="4"/>
       <c r="V366" s="4"/>
@@ -21893,7 +22083,9 @@
       <c r="AC366" s="4"/>
       <c r="AD366" s="4"/>
       <c r="AE366" s="4"/>
-      <c r="AF366" s="4"/>
+      <c r="AF366" s="4">
+        <v>1</v>
+      </c>
       <c r="AG366" s="4"/>
       <c r="AH366" s="4"/>
       <c r="AI366" s="4"/>
@@ -22010,16 +22202,24 @@
       <c r="T369" s="4"/>
       <c r="U369" s="4"/>
       <c r="V369" s="4"/>
-      <c r="W369" s="4"/>
-      <c r="X369" s="4"/>
-      <c r="Y369" s="4"/>
+      <c r="W369" s="4">
+        <v>1</v>
+      </c>
+      <c r="X369" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y369" s="4">
+        <v>1</v>
+      </c>
       <c r="Z369" s="4"/>
       <c r="AA369" s="4"/>
       <c r="AB369" s="4"/>
       <c r="AC369" s="4"/>
       <c r="AD369" s="4"/>
       <c r="AE369" s="4"/>
-      <c r="AF369" s="4"/>
+      <c r="AF369" s="4">
+        <v>1</v>
+      </c>
       <c r="AG369" s="4"/>
       <c r="AH369" s="4"/>
       <c r="AI369" s="4"/>
@@ -22128,11 +22328,21 @@
       <c r="L373" s="4"/>
       <c r="M373" s="4"/>
       <c r="N373" s="4"/>
-      <c r="O373" s="4"/>
-      <c r="P373" s="4"/>
-      <c r="Q373" s="4"/>
-      <c r="R373" s="4"/>
-      <c r="S373" s="4"/>
+      <c r="O373" s="4">
+        <v>0.5524</v>
+      </c>
+      <c r="P373" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Q373" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="R373" s="4">
+        <v>0.31180000000000008</v>
+      </c>
+      <c r="S373" s="4">
+        <v>0.28720000000000001</v>
+      </c>
       <c r="T373" s="4"/>
       <c r="U373" s="4"/>
       <c r="V373" s="4"/>
@@ -22254,11 +22464,21 @@
       <c r="L376" s="4"/>
       <c r="M376" s="4"/>
       <c r="N376" s="4"/>
-      <c r="O376" s="4"/>
-      <c r="P376" s="4"/>
-      <c r="Q376" s="4"/>
-      <c r="R376" s="4"/>
-      <c r="S376" s="4"/>
+      <c r="O376" s="4">
+        <v>0.5524</v>
+      </c>
+      <c r="P376" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Q376" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="R376" s="4">
+        <v>0.31180000000000008</v>
+      </c>
+      <c r="S376" s="4">
+        <v>0.28720000000000001</v>
+      </c>
       <c r="T376" s="4"/>
       <c r="U376" s="4"/>
       <c r="V376" s="4"/>
@@ -22380,11 +22600,21 @@
       <c r="L379" s="4"/>
       <c r="M379" s="4"/>
       <c r="N379" s="4"/>
-      <c r="O379" s="4"/>
-      <c r="P379" s="4"/>
-      <c r="Q379" s="4"/>
-      <c r="R379" s="4"/>
-      <c r="S379" s="4"/>
+      <c r="O379" s="4">
+        <v>0.5524</v>
+      </c>
+      <c r="P379" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Q379" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="R379" s="4">
+        <v>0.31180000000000008</v>
+      </c>
+      <c r="S379" s="4">
+        <v>0.28720000000000001</v>
+      </c>
       <c r="T379" s="4"/>
       <c r="U379" s="4"/>
       <c r="V379" s="4"/>
@@ -22506,11 +22736,21 @@
       <c r="L382" s="4"/>
       <c r="M382" s="4"/>
       <c r="N382" s="4"/>
-      <c r="O382" s="4"/>
-      <c r="P382" s="4"/>
-      <c r="Q382" s="4"/>
-      <c r="R382" s="4"/>
-      <c r="S382" s="4"/>
+      <c r="O382" s="4">
+        <v>0.5524</v>
+      </c>
+      <c r="P382" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Q382" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="R382" s="4">
+        <v>0.31180000000000008</v>
+      </c>
+      <c r="S382" s="4">
+        <v>0.28720000000000001</v>
+      </c>
       <c r="T382" s="4"/>
       <c r="U382" s="4"/>
       <c r="V382" s="4"/>
@@ -22640,9 +22880,15 @@
       <c r="T385" s="4"/>
       <c r="U385" s="4"/>
       <c r="V385" s="4"/>
-      <c r="W385" s="4"/>
-      <c r="X385" s="4"/>
-      <c r="Y385" s="4"/>
+      <c r="W385" s="4">
+        <v>0.44720000000000004</v>
+      </c>
+      <c r="X385" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Y385" s="4">
+        <v>0.14529999999999998</v>
+      </c>
       <c r="Z385" s="4"/>
       <c r="AA385" s="4"/>
       <c r="AB385" s="4"/>
@@ -22766,9 +23012,15 @@
       <c r="T388" s="4"/>
       <c r="U388" s="4"/>
       <c r="V388" s="4"/>
-      <c r="W388" s="4"/>
-      <c r="X388" s="4"/>
-      <c r="Y388" s="4"/>
+      <c r="W388" s="4">
+        <v>0.44720000000000004</v>
+      </c>
+      <c r="X388" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Y388" s="4">
+        <v>0.14529999999999998</v>
+      </c>
       <c r="Z388" s="4"/>
       <c r="AA388" s="4"/>
       <c r="AB388" s="4"/>
@@ -22884,11 +23136,21 @@
       <c r="L391" s="4"/>
       <c r="M391" s="4"/>
       <c r="N391" s="4"/>
-      <c r="O391" s="4"/>
-      <c r="P391" s="4"/>
-      <c r="Q391" s="4"/>
-      <c r="R391" s="4"/>
-      <c r="S391" s="4"/>
+      <c r="O391" s="4">
+        <v>0.5524</v>
+      </c>
+      <c r="P391" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Q391" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="R391" s="4">
+        <v>0.31180000000000008</v>
+      </c>
+      <c r="S391" s="4">
+        <v>0.28720000000000001</v>
+      </c>
       <c r="T391" s="4"/>
       <c r="U391" s="4"/>
       <c r="V391" s="4"/>
@@ -22898,7 +23160,9 @@
       <c r="Z391" s="4"/>
       <c r="AA391" s="4"/>
       <c r="AB391" s="4"/>
-      <c r="AC391" s="4"/>
+      <c r="AC391" s="4">
+        <v>1</v>
+      </c>
       <c r="AD391" s="4"/>
       <c r="AE391" s="4"/>
       <c r="AF391" s="4"/>
@@ -23018,13 +23282,21 @@
       <c r="T394" s="4"/>
       <c r="U394" s="4"/>
       <c r="V394" s="4"/>
-      <c r="W394" s="4"/>
-      <c r="X394" s="4"/>
-      <c r="Y394" s="4"/>
+      <c r="W394" s="4">
+        <v>0.44720000000000004</v>
+      </c>
+      <c r="X394" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Y394" s="4">
+        <v>0.14529999999999998</v>
+      </c>
       <c r="Z394" s="4"/>
       <c r="AA394" s="4"/>
       <c r="AB394" s="4"/>
-      <c r="AC394" s="4"/>
+      <c r="AC394" s="4">
+        <v>1</v>
+      </c>
       <c r="AD394" s="4"/>
       <c r="AE394" s="4"/>
       <c r="AF394" s="4"/>
@@ -23388,11 +23660,21 @@
       <c r="L403" s="4"/>
       <c r="M403" s="4"/>
       <c r="N403" s="4"/>
-      <c r="O403" s="4"/>
-      <c r="P403" s="4"/>
-      <c r="Q403" s="4"/>
-      <c r="R403" s="4"/>
-      <c r="S403" s="4"/>
+      <c r="O403" s="4">
+        <v>0.5524</v>
+      </c>
+      <c r="P403" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Q403" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="R403" s="4">
+        <v>0.31180000000000008</v>
+      </c>
+      <c r="S403" s="4">
+        <v>0.28720000000000001</v>
+      </c>
       <c r="T403" s="4"/>
       <c r="U403" s="4"/>
       <c r="V403" s="4"/>
@@ -23405,7 +23687,9 @@
       <c r="AC403" s="4"/>
       <c r="AD403" s="4"/>
       <c r="AE403" s="4"/>
-      <c r="AF403" s="4"/>
+      <c r="AF403" s="4">
+        <v>1</v>
+      </c>
       <c r="AG403" s="4"/>
       <c r="AH403" s="4"/>
       <c r="AI403" s="4"/>
@@ -23522,16 +23806,24 @@
       <c r="T406" s="4"/>
       <c r="U406" s="4"/>
       <c r="V406" s="4"/>
-      <c r="W406" s="4"/>
-      <c r="X406" s="4"/>
-      <c r="Y406" s="4"/>
+      <c r="W406" s="4">
+        <v>0.44720000000000004</v>
+      </c>
+      <c r="X406" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Y406" s="4">
+        <v>0.14529999999999998</v>
+      </c>
       <c r="Z406" s="4"/>
       <c r="AA406" s="4"/>
       <c r="AB406" s="4"/>
       <c r="AC406" s="4"/>
       <c r="AD406" s="4"/>
       <c r="AE406" s="4"/>
-      <c r="AF406" s="4"/>
+      <c r="AF406" s="4">
+        <v>1</v>
+      </c>
       <c r="AG406" s="4"/>
       <c r="AH406" s="4"/>
       <c r="AI406" s="4"/>
@@ -23640,11 +23932,21 @@
       <c r="L410" s="4"/>
       <c r="M410" s="4"/>
       <c r="N410" s="4"/>
-      <c r="O410" s="4"/>
-      <c r="P410" s="4"/>
-      <c r="Q410" s="4"/>
-      <c r="R410" s="4"/>
-      <c r="S410" s="4"/>
+      <c r="O410" s="4">
+        <v>0.39816945906675694</v>
+      </c>
+      <c r="P410" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Q410" s="4">
+        <v>0.52714374529406949</v>
+      </c>
+      <c r="R410" s="4">
+        <v>0.68592239052443116</v>
+      </c>
+      <c r="S410" s="4">
+        <v>0.74456761445968844</v>
+      </c>
       <c r="T410" s="4"/>
       <c r="U410" s="4"/>
       <c r="V410" s="4"/>
@@ -23766,11 +24068,21 @@
       <c r="L413" s="4"/>
       <c r="M413" s="4"/>
       <c r="N413" s="4"/>
-      <c r="O413" s="4"/>
-      <c r="P413" s="4"/>
-      <c r="Q413" s="4"/>
-      <c r="R413" s="4"/>
-      <c r="S413" s="4"/>
+      <c r="O413" s="4">
+        <v>0.39816945906675694</v>
+      </c>
+      <c r="P413" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Q413" s="4">
+        <v>0.52714374529406949</v>
+      </c>
+      <c r="R413" s="4">
+        <v>0.68592239052443116</v>
+      </c>
+      <c r="S413" s="4">
+        <v>0.74456761445968844</v>
+      </c>
       <c r="T413" s="4"/>
       <c r="U413" s="4"/>
       <c r="V413" s="4"/>
@@ -23892,11 +24204,21 @@
       <c r="L416" s="4"/>
       <c r="M416" s="4"/>
       <c r="N416" s="4"/>
-      <c r="O416" s="4"/>
-      <c r="P416" s="4"/>
-      <c r="Q416" s="4"/>
-      <c r="R416" s="4"/>
-      <c r="S416" s="4"/>
+      <c r="O416" s="4">
+        <v>0.39816945906675694</v>
+      </c>
+      <c r="P416" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Q416" s="4">
+        <v>0.52714374529406949</v>
+      </c>
+      <c r="R416" s="4">
+        <v>0.68592239052443116</v>
+      </c>
+      <c r="S416" s="4">
+        <v>0.74456761445968844</v>
+      </c>
       <c r="T416" s="4"/>
       <c r="U416" s="4"/>
       <c r="V416" s="4"/>
@@ -24018,11 +24340,21 @@
       <c r="L419" s="4"/>
       <c r="M419" s="4"/>
       <c r="N419" s="4"/>
-      <c r="O419" s="4"/>
-      <c r="P419" s="4"/>
-      <c r="Q419" s="4"/>
-      <c r="R419" s="4"/>
-      <c r="S419" s="4"/>
+      <c r="O419" s="4">
+        <v>0.39816945906675694</v>
+      </c>
+      <c r="P419" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Q419" s="4">
+        <v>0.52714374529406949</v>
+      </c>
+      <c r="R419" s="4">
+        <v>0.68592239052443116</v>
+      </c>
+      <c r="S419" s="4">
+        <v>0.74456761445968844</v>
+      </c>
       <c r="T419" s="4"/>
       <c r="U419" s="4"/>
       <c r="V419" s="4"/>
@@ -24152,9 +24484,15 @@
       <c r="T422" s="4"/>
       <c r="U422" s="4"/>
       <c r="V422" s="4"/>
-      <c r="W422" s="4"/>
-      <c r="X422" s="4"/>
-      <c r="Y422" s="4"/>
+      <c r="W422" s="4">
+        <v>0.33411712741654032</v>
+      </c>
+      <c r="X422" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Y422" s="4">
+        <v>0.61708679020377177</v>
+      </c>
       <c r="Z422" s="4"/>
       <c r="AA422" s="4"/>
       <c r="AB422" s="4"/>
@@ -24278,9 +24616,15 @@
       <c r="T425" s="4"/>
       <c r="U425" s="4"/>
       <c r="V425" s="4"/>
-      <c r="W425" s="4"/>
-      <c r="X425" s="4"/>
-      <c r="Y425" s="4"/>
+      <c r="W425" s="4">
+        <v>0.33411712741654032</v>
+      </c>
+      <c r="X425" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Y425" s="4">
+        <v>0.61708679020377177</v>
+      </c>
       <c r="Z425" s="4"/>
       <c r="AA425" s="4"/>
       <c r="AB425" s="4"/>
@@ -24396,11 +24740,21 @@
       <c r="L428" s="4"/>
       <c r="M428" s="4"/>
       <c r="N428" s="4"/>
-      <c r="O428" s="4"/>
-      <c r="P428" s="4"/>
-      <c r="Q428" s="4"/>
-      <c r="R428" s="4"/>
-      <c r="S428" s="4"/>
+      <c r="O428" s="4">
+        <v>0.39816945906675694</v>
+      </c>
+      <c r="P428" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Q428" s="4">
+        <v>0.52714374529406949</v>
+      </c>
+      <c r="R428" s="4">
+        <v>0.68592239052443116</v>
+      </c>
+      <c r="S428" s="4">
+        <v>0.74456761445968844</v>
+      </c>
       <c r="T428" s="4"/>
       <c r="U428" s="4"/>
       <c r="V428" s="4"/>
@@ -24410,7 +24764,9 @@
       <c r="Z428" s="4"/>
       <c r="AA428" s="4"/>
       <c r="AB428" s="4"/>
-      <c r="AC428" s="4"/>
+      <c r="AC428" s="4">
+        <v>0</v>
+      </c>
       <c r="AD428" s="4"/>
       <c r="AE428" s="4"/>
       <c r="AF428" s="4"/>
@@ -24530,13 +24886,21 @@
       <c r="T431" s="4"/>
       <c r="U431" s="4"/>
       <c r="V431" s="4"/>
-      <c r="W431" s="4"/>
-      <c r="X431" s="4"/>
-      <c r="Y431" s="4"/>
+      <c r="W431" s="4">
+        <v>0.33411712741654032</v>
+      </c>
+      <c r="X431" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Y431" s="4">
+        <v>0.61708679020377177</v>
+      </c>
       <c r="Z431" s="4"/>
       <c r="AA431" s="4"/>
       <c r="AB431" s="4"/>
-      <c r="AC431" s="4"/>
+      <c r="AC431" s="4">
+        <v>0</v>
+      </c>
       <c r="AD431" s="4"/>
       <c r="AE431" s="4"/>
       <c r="AF431" s="4"/>
@@ -24900,11 +25264,21 @@
       <c r="L440" s="4"/>
       <c r="M440" s="4"/>
       <c r="N440" s="4"/>
-      <c r="O440" s="4"/>
-      <c r="P440" s="4"/>
-      <c r="Q440" s="4"/>
-      <c r="R440" s="4"/>
-      <c r="S440" s="4"/>
+      <c r="O440" s="4">
+        <v>0.39816945906675694</v>
+      </c>
+      <c r="P440" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Q440" s="4">
+        <v>0.52714374529406949</v>
+      </c>
+      <c r="R440" s="4">
+        <v>0.68592239052443116</v>
+      </c>
+      <c r="S440" s="4">
+        <v>0.74456761445968844</v>
+      </c>
       <c r="T440" s="4"/>
       <c r="U440" s="4"/>
       <c r="V440" s="4"/>
@@ -24917,7 +25291,9 @@
       <c r="AC440" s="4"/>
       <c r="AD440" s="4"/>
       <c r="AE440" s="4"/>
-      <c r="AF440" s="4"/>
+      <c r="AF440" s="4">
+        <v>0</v>
+      </c>
       <c r="AG440" s="4"/>
       <c r="AH440" s="4"/>
       <c r="AI440" s="4"/>
@@ -25034,16 +25410,24 @@
       <c r="T443" s="4"/>
       <c r="U443" s="4"/>
       <c r="V443" s="4"/>
-      <c r="W443" s="4"/>
-      <c r="X443" s="4"/>
-      <c r="Y443" s="4"/>
+      <c r="W443" s="4">
+        <v>0.33411712741654032</v>
+      </c>
+      <c r="X443" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Y443" s="4">
+        <v>0.61708679020377177</v>
+      </c>
       <c r="Z443" s="4"/>
       <c r="AA443" s="4"/>
       <c r="AB443" s="4"/>
       <c r="AC443" s="4"/>
       <c r="AD443" s="4"/>
       <c r="AE443" s="4"/>
-      <c r="AF443" s="4"/>
+      <c r="AF443" s="4">
+        <v>0</v>
+      </c>
       <c r="AG443" s="4"/>
       <c r="AH443" s="4"/>
       <c r="AI443" s="4"/>
@@ -26751,8 +27135,12 @@
       <c r="Q484" s="4"/>
       <c r="R484" s="4"/>
       <c r="S484" s="4"/>
-      <c r="T484" s="4"/>
-      <c r="U484" s="4"/>
+      <c r="T484" s="4">
+        <v>1</v>
+      </c>
+      <c r="U484" s="4">
+        <v>1</v>
+      </c>
       <c r="V484" s="4"/>
       <c r="W484" s="4"/>
       <c r="X484" s="4"/>
@@ -26877,8 +27265,12 @@
       <c r="Q487" s="4"/>
       <c r="R487" s="4"/>
       <c r="S487" s="4"/>
-      <c r="T487" s="4"/>
-      <c r="U487" s="4"/>
+      <c r="T487" s="4">
+        <v>1</v>
+      </c>
+      <c r="U487" s="4">
+        <v>1</v>
+      </c>
       <c r="V487" s="4"/>
       <c r="W487" s="4"/>
       <c r="X487" s="4"/>
@@ -27003,8 +27395,12 @@
       <c r="Q490" s="4"/>
       <c r="R490" s="4"/>
       <c r="S490" s="4"/>
-      <c r="T490" s="4"/>
-      <c r="U490" s="4"/>
+      <c r="T490" s="4">
+        <v>1</v>
+      </c>
+      <c r="U490" s="4">
+        <v>1</v>
+      </c>
       <c r="V490" s="4"/>
       <c r="W490" s="4"/>
       <c r="X490" s="4"/>
@@ -27129,8 +27525,12 @@
       <c r="Q493" s="4"/>
       <c r="R493" s="4"/>
       <c r="S493" s="4"/>
-      <c r="T493" s="4"/>
-      <c r="U493" s="4"/>
+      <c r="T493" s="4">
+        <v>1</v>
+      </c>
+      <c r="U493" s="4">
+        <v>1</v>
+      </c>
       <c r="V493" s="4"/>
       <c r="W493" s="4"/>
       <c r="X493" s="4"/>
@@ -27261,8 +27661,12 @@
       <c r="W496" s="4"/>
       <c r="X496" s="4"/>
       <c r="Y496" s="4"/>
-      <c r="Z496" s="4"/>
-      <c r="AA496" s="4"/>
+      <c r="Z496" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA496" s="4">
+        <v>1</v>
+      </c>
       <c r="AB496" s="4"/>
       <c r="AC496" s="4"/>
       <c r="AD496" s="4"/>
@@ -27387,8 +27791,12 @@
       <c r="W499" s="4"/>
       <c r="X499" s="4"/>
       <c r="Y499" s="4"/>
-      <c r="Z499" s="4"/>
-      <c r="AA499" s="4"/>
+      <c r="Z499" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA499" s="4">
+        <v>1</v>
+      </c>
       <c r="AB499" s="4"/>
       <c r="AC499" s="4"/>
       <c r="AD499" s="4"/>
@@ -27507,8 +27915,12 @@
       <c r="Q502" s="4"/>
       <c r="R502" s="4"/>
       <c r="S502" s="4"/>
-      <c r="T502" s="4"/>
-      <c r="U502" s="4"/>
+      <c r="T502" s="4">
+        <v>1</v>
+      </c>
+      <c r="U502" s="4">
+        <v>1</v>
+      </c>
       <c r="V502" s="4"/>
       <c r="W502" s="4"/>
       <c r="X502" s="4"/>
@@ -27517,7 +27929,9 @@
       <c r="AA502" s="4"/>
       <c r="AB502" s="4"/>
       <c r="AC502" s="4"/>
-      <c r="AD502" s="4"/>
+      <c r="AD502" s="4">
+        <v>1</v>
+      </c>
       <c r="AE502" s="4"/>
       <c r="AF502" s="4"/>
       <c r="AG502" s="4"/>
@@ -27639,11 +28053,17 @@
       <c r="W505" s="4"/>
       <c r="X505" s="4"/>
       <c r="Y505" s="4"/>
-      <c r="Z505" s="4"/>
-      <c r="AA505" s="4"/>
+      <c r="Z505" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA505" s="4">
+        <v>1</v>
+      </c>
       <c r="AB505" s="4"/>
       <c r="AC505" s="4"/>
-      <c r="AD505" s="4"/>
+      <c r="AD505" s="4">
+        <v>1</v>
+      </c>
       <c r="AE505" s="4"/>
       <c r="AF505" s="4"/>
       <c r="AG505" s="4"/>
@@ -28011,8 +28431,12 @@
       <c r="Q514" s="4"/>
       <c r="R514" s="4"/>
       <c r="S514" s="4"/>
-      <c r="T514" s="4"/>
-      <c r="U514" s="4"/>
+      <c r="T514" s="4">
+        <v>1</v>
+      </c>
+      <c r="U514" s="4">
+        <v>1</v>
+      </c>
       <c r="V514" s="4"/>
       <c r="W514" s="4"/>
       <c r="X514" s="4"/>
@@ -28024,7 +28448,9 @@
       <c r="AD514" s="4"/>
       <c r="AE514" s="4"/>
       <c r="AF514" s="4"/>
-      <c r="AG514" s="4"/>
+      <c r="AG514" s="4">
+        <v>1</v>
+      </c>
       <c r="AH514" s="4"/>
       <c r="AI514" s="4"/>
       <c r="AJ514" s="4"/>
@@ -28143,14 +28569,20 @@
       <c r="W517" s="4"/>
       <c r="X517" s="4"/>
       <c r="Y517" s="4"/>
-      <c r="Z517" s="4"/>
-      <c r="AA517" s="4"/>
+      <c r="Z517" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA517" s="4">
+        <v>1</v>
+      </c>
       <c r="AB517" s="4"/>
       <c r="AC517" s="4"/>
       <c r="AD517" s="4"/>
       <c r="AE517" s="4"/>
       <c r="AF517" s="4"/>
-      <c r="AG517" s="4"/>
+      <c r="AG517" s="4">
+        <v>1</v>
+      </c>
       <c r="AH517" s="4"/>
       <c r="AI517" s="4"/>
       <c r="AJ517" s="4"/>
@@ -28263,8 +28695,12 @@
       <c r="Q521" s="4"/>
       <c r="R521" s="4"/>
       <c r="S521" s="4"/>
-      <c r="T521" s="4"/>
-      <c r="U521" s="4"/>
+      <c r="T521" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="U521" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="V521" s="4"/>
       <c r="W521" s="4"/>
       <c r="X521" s="4"/>
@@ -28389,8 +28825,12 @@
       <c r="Q524" s="4"/>
       <c r="R524" s="4"/>
       <c r="S524" s="4"/>
-      <c r="T524" s="4"/>
-      <c r="U524" s="4"/>
+      <c r="T524" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="U524" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="V524" s="4"/>
       <c r="W524" s="4"/>
       <c r="X524" s="4"/>
@@ -28515,8 +28955,12 @@
       <c r="Q527" s="4"/>
       <c r="R527" s="4"/>
       <c r="S527" s="4"/>
-      <c r="T527" s="4"/>
-      <c r="U527" s="4"/>
+      <c r="T527" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="U527" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="V527" s="4"/>
       <c r="W527" s="4"/>
       <c r="X527" s="4"/>
@@ -28641,8 +29085,12 @@
       <c r="Q530" s="4"/>
       <c r="R530" s="4"/>
       <c r="S530" s="4"/>
-      <c r="T530" s="4"/>
-      <c r="U530" s="4"/>
+      <c r="T530" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="U530" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="V530" s="4"/>
       <c r="W530" s="4"/>
       <c r="X530" s="4"/>
@@ -28773,8 +29221,12 @@
       <c r="W533" s="4"/>
       <c r="X533" s="4"/>
       <c r="Y533" s="4"/>
-      <c r="Z533" s="4"/>
-      <c r="AA533" s="4"/>
+      <c r="Z533" s="4">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="AA533" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="AB533" s="4"/>
       <c r="AC533" s="4"/>
       <c r="AD533" s="4"/>
@@ -28899,8 +29351,12 @@
       <c r="W536" s="4"/>
       <c r="X536" s="4"/>
       <c r="Y536" s="4"/>
-      <c r="Z536" s="4"/>
-      <c r="AA536" s="4"/>
+      <c r="Z536" s="4">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="AA536" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="AB536" s="4"/>
       <c r="AC536" s="4"/>
       <c r="AD536" s="4"/>
@@ -29019,8 +29475,12 @@
       <c r="Q539" s="4"/>
       <c r="R539" s="4"/>
       <c r="S539" s="4"/>
-      <c r="T539" s="4"/>
-      <c r="U539" s="4"/>
+      <c r="T539" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="U539" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="V539" s="4"/>
       <c r="W539" s="4"/>
       <c r="X539" s="4"/>
@@ -29029,7 +29489,9 @@
       <c r="AA539" s="4"/>
       <c r="AB539" s="4"/>
       <c r="AC539" s="4"/>
-      <c r="AD539" s="4"/>
+      <c r="AD539" s="4">
+        <v>1</v>
+      </c>
       <c r="AE539" s="4"/>
       <c r="AF539" s="4"/>
       <c r="AG539" s="4"/>
@@ -29151,11 +29613,17 @@
       <c r="W542" s="4"/>
       <c r="X542" s="4"/>
       <c r="Y542" s="4"/>
-      <c r="Z542" s="4"/>
-      <c r="AA542" s="4"/>
+      <c r="Z542" s="4">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="AA542" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="AB542" s="4"/>
       <c r="AC542" s="4"/>
-      <c r="AD542" s="4"/>
+      <c r="AD542" s="4">
+        <v>1</v>
+      </c>
       <c r="AE542" s="4"/>
       <c r="AF542" s="4"/>
       <c r="AG542" s="4"/>
@@ -29523,8 +29991,12 @@
       <c r="Q551" s="4"/>
       <c r="R551" s="4"/>
       <c r="S551" s="4"/>
-      <c r="T551" s="4"/>
-      <c r="U551" s="4"/>
+      <c r="T551" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="U551" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="V551" s="4"/>
       <c r="W551" s="4"/>
       <c r="X551" s="4"/>
@@ -29536,7 +30008,9 @@
       <c r="AD551" s="4"/>
       <c r="AE551" s="4"/>
       <c r="AF551" s="4"/>
-      <c r="AG551" s="4"/>
+      <c r="AG551" s="4">
+        <v>1</v>
+      </c>
       <c r="AH551" s="4"/>
       <c r="AI551" s="4"/>
       <c r="AJ551" s="4"/>
@@ -29655,14 +30129,20 @@
       <c r="W554" s="4"/>
       <c r="X554" s="4"/>
       <c r="Y554" s="4"/>
-      <c r="Z554" s="4"/>
-      <c r="AA554" s="4"/>
+      <c r="Z554" s="4">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="AA554" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="AB554" s="4"/>
       <c r="AC554" s="4"/>
       <c r="AD554" s="4"/>
       <c r="AE554" s="4"/>
       <c r="AF554" s="4"/>
-      <c r="AG554" s="4"/>
+      <c r="AG554" s="4">
+        <v>1</v>
+      </c>
       <c r="AH554" s="4"/>
       <c r="AI554" s="4"/>
       <c r="AJ554" s="4"/>
@@ -29775,8 +30255,12 @@
       <c r="Q558" s="4"/>
       <c r="R558" s="4"/>
       <c r="S558" s="4"/>
-      <c r="T558" s="4"/>
-      <c r="U558" s="4"/>
+      <c r="T558" s="4">
+        <v>0.38926274061590116</v>
+      </c>
+      <c r="U558" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="V558" s="4"/>
       <c r="W558" s="4"/>
       <c r="X558" s="4"/>
@@ -29901,8 +30385,12 @@
       <c r="Q561" s="4"/>
       <c r="R561" s="4"/>
       <c r="S561" s="4"/>
-      <c r="T561" s="4"/>
-      <c r="U561" s="4"/>
+      <c r="T561" s="4">
+        <v>0.38926274061590116</v>
+      </c>
+      <c r="U561" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="V561" s="4"/>
       <c r="W561" s="4"/>
       <c r="X561" s="4"/>
@@ -30027,8 +30515,12 @@
       <c r="Q564" s="4"/>
       <c r="R564" s="4"/>
       <c r="S564" s="4"/>
-      <c r="T564" s="4"/>
-      <c r="U564" s="4"/>
+      <c r="T564" s="4">
+        <v>0.38926274061590116</v>
+      </c>
+      <c r="U564" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="V564" s="4"/>
       <c r="W564" s="4"/>
       <c r="X564" s="4"/>
@@ -30153,8 +30645,12 @@
       <c r="Q567" s="4"/>
       <c r="R567" s="4"/>
       <c r="S567" s="4"/>
-      <c r="T567" s="4"/>
-      <c r="U567" s="4"/>
+      <c r="T567" s="4">
+        <v>0.38926274061590116</v>
+      </c>
+      <c r="U567" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="V567" s="4"/>
       <c r="W567" s="4"/>
       <c r="X567" s="4"/>
@@ -30285,8 +30781,12 @@
       <c r="W570" s="4"/>
       <c r="X570" s="4"/>
       <c r="Y570" s="4"/>
-      <c r="Z570" s="4"/>
-      <c r="AA570" s="4"/>
+      <c r="Z570" s="4">
+        <v>0.2344936316398144</v>
+      </c>
+      <c r="AA570" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="AB570" s="4"/>
       <c r="AC570" s="4"/>
       <c r="AD570" s="4"/>
@@ -30411,8 +30911,12 @@
       <c r="W573" s="4"/>
       <c r="X573" s="4"/>
       <c r="Y573" s="4"/>
-      <c r="Z573" s="4"/>
-      <c r="AA573" s="4"/>
+      <c r="Z573" s="4">
+        <v>0.2344936316398144</v>
+      </c>
+      <c r="AA573" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="AB573" s="4"/>
       <c r="AC573" s="4"/>
       <c r="AD573" s="4"/>
@@ -30531,8 +31035,12 @@
       <c r="Q576" s="4"/>
       <c r="R576" s="4"/>
       <c r="S576" s="4"/>
-      <c r="T576" s="4"/>
-      <c r="U576" s="4"/>
+      <c r="T576" s="4">
+        <v>0.38926274061590116</v>
+      </c>
+      <c r="U576" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="V576" s="4"/>
       <c r="W576" s="4"/>
       <c r="X576" s="4"/>
@@ -30541,7 +31049,9 @@
       <c r="AA576" s="4"/>
       <c r="AB576" s="4"/>
       <c r="AC576" s="4"/>
-      <c r="AD576" s="4"/>
+      <c r="AD576" s="4">
+        <v>0</v>
+      </c>
       <c r="AE576" s="4"/>
       <c r="AF576" s="4"/>
       <c r="AG576" s="4"/>
@@ -30663,11 +31173,17 @@
       <c r="W579" s="4"/>
       <c r="X579" s="4"/>
       <c r="Y579" s="4"/>
-      <c r="Z579" s="4"/>
-      <c r="AA579" s="4"/>
+      <c r="Z579" s="4">
+        <v>0.2344936316398144</v>
+      </c>
+      <c r="AA579" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="AB579" s="4"/>
       <c r="AC579" s="4"/>
-      <c r="AD579" s="4"/>
+      <c r="AD579" s="4">
+        <v>0</v>
+      </c>
       <c r="AE579" s="4"/>
       <c r="AF579" s="4"/>
       <c r="AG579" s="4"/>
@@ -31035,8 +31551,12 @@
       <c r="Q588" s="4"/>
       <c r="R588" s="4"/>
       <c r="S588" s="4"/>
-      <c r="T588" s="4"/>
-      <c r="U588" s="4"/>
+      <c r="T588" s="4">
+        <v>0.38926274061590116</v>
+      </c>
+      <c r="U588" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="V588" s="4"/>
       <c r="W588" s="4"/>
       <c r="X588" s="4"/>
@@ -31048,7 +31568,9 @@
       <c r="AD588" s="4"/>
       <c r="AE588" s="4"/>
       <c r="AF588" s="4"/>
-      <c r="AG588" s="4"/>
+      <c r="AG588" s="4">
+        <v>0</v>
+      </c>
       <c r="AH588" s="4"/>
       <c r="AI588" s="4"/>
       <c r="AJ588" s="4"/>
@@ -31167,14 +31689,20 @@
       <c r="W591" s="4"/>
       <c r="X591" s="4"/>
       <c r="Y591" s="4"/>
-      <c r="Z591" s="4"/>
-      <c r="AA591" s="4"/>
+      <c r="Z591" s="4">
+        <v>0.2344936316398144</v>
+      </c>
+      <c r="AA591" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="AB591" s="4"/>
       <c r="AC591" s="4"/>
       <c r="AD591" s="4"/>
       <c r="AE591" s="4"/>
       <c r="AF591" s="4"/>
-      <c r="AG591" s="4"/>
+      <c r="AG591" s="4">
+        <v>0</v>
+      </c>
       <c r="AH591" s="4"/>
       <c r="AI591" s="4"/>
       <c r="AJ591" s="4"/>
@@ -32875,7 +33403,9 @@
       <c r="K632" s="4"/>
       <c r="L632" s="4"/>
       <c r="M632" s="4"/>
-      <c r="N632" s="4"/>
+      <c r="N632" s="4">
+        <v>1</v>
+      </c>
       <c r="O632" s="4"/>
       <c r="P632" s="4"/>
       <c r="Q632" s="4"/>
@@ -33001,7 +33531,9 @@
       <c r="K635" s="4"/>
       <c r="L635" s="4"/>
       <c r="M635" s="4"/>
-      <c r="N635" s="4"/>
+      <c r="N635" s="4">
+        <v>1</v>
+      </c>
       <c r="O635" s="4"/>
       <c r="P635" s="4"/>
       <c r="Q635" s="4"/>
@@ -33127,7 +33659,9 @@
       <c r="K638" s="4"/>
       <c r="L638" s="4"/>
       <c r="M638" s="4"/>
-      <c r="N638" s="4"/>
+      <c r="N638" s="4">
+        <v>1</v>
+      </c>
       <c r="O638" s="4"/>
       <c r="P638" s="4"/>
       <c r="Q638" s="4"/>
@@ -33253,7 +33787,9 @@
       <c r="K641" s="4"/>
       <c r="L641" s="4"/>
       <c r="M641" s="4"/>
-      <c r="N641" s="4"/>
+      <c r="N641" s="4">
+        <v>1</v>
+      </c>
       <c r="O641" s="4"/>
       <c r="P641" s="4"/>
       <c r="Q641" s="4"/>
@@ -33387,7 +33923,9 @@
       <c r="S644" s="4"/>
       <c r="T644" s="4"/>
       <c r="U644" s="4"/>
-      <c r="V644" s="4"/>
+      <c r="V644" s="4">
+        <v>1</v>
+      </c>
       <c r="W644" s="4"/>
       <c r="X644" s="4"/>
       <c r="Y644" s="4"/>
@@ -33513,7 +34051,9 @@
       <c r="S647" s="4"/>
       <c r="T647" s="4"/>
       <c r="U647" s="4"/>
-      <c r="V647" s="4"/>
+      <c r="V647" s="4">
+        <v>1</v>
+      </c>
       <c r="W647" s="4"/>
       <c r="X647" s="4"/>
       <c r="Y647" s="4"/>
@@ -33631,7 +34171,9 @@
       <c r="K650" s="4"/>
       <c r="L650" s="4"/>
       <c r="M650" s="4"/>
-      <c r="N650" s="4"/>
+      <c r="N650" s="4">
+        <v>1</v>
+      </c>
       <c r="O650" s="4"/>
       <c r="P650" s="4"/>
       <c r="Q650" s="4"/>
@@ -33645,7 +34187,9 @@
       <c r="Y650" s="4"/>
       <c r="Z650" s="4"/>
       <c r="AA650" s="4"/>
-      <c r="AB650" s="4"/>
+      <c r="AB650" s="4">
+        <v>1</v>
+      </c>
       <c r="AC650" s="4"/>
       <c r="AD650" s="4"/>
       <c r="AE650" s="4"/>
@@ -33765,13 +34309,17 @@
       <c r="S653" s="4"/>
       <c r="T653" s="4"/>
       <c r="U653" s="4"/>
-      <c r="V653" s="4"/>
+      <c r="V653" s="4">
+        <v>1</v>
+      </c>
       <c r="W653" s="4"/>
       <c r="X653" s="4"/>
       <c r="Y653" s="4"/>
       <c r="Z653" s="4"/>
       <c r="AA653" s="4"/>
-      <c r="AB653" s="4"/>
+      <c r="AB653" s="4">
+        <v>1</v>
+      </c>
       <c r="AC653" s="4"/>
       <c r="AD653" s="4"/>
       <c r="AE653" s="4"/>
@@ -34135,7 +34683,9 @@
       <c r="K662" s="4"/>
       <c r="L662" s="4"/>
       <c r="M662" s="4"/>
-      <c r="N662" s="4"/>
+      <c r="N662" s="4">
+        <v>1</v>
+      </c>
       <c r="O662" s="4"/>
       <c r="P662" s="4"/>
       <c r="Q662" s="4"/>
@@ -34152,7 +34702,9 @@
       <c r="AB662" s="4"/>
       <c r="AC662" s="4"/>
       <c r="AD662" s="4"/>
-      <c r="AE662" s="4"/>
+      <c r="AE662" s="4">
+        <v>1</v>
+      </c>
       <c r="AF662" s="4"/>
       <c r="AG662" s="4"/>
       <c r="AH662" s="4"/>
@@ -34269,7 +34821,9 @@
       <c r="S665" s="4"/>
       <c r="T665" s="4"/>
       <c r="U665" s="4"/>
-      <c r="V665" s="4"/>
+      <c r="V665" s="4">
+        <v>1</v>
+      </c>
       <c r="W665" s="4"/>
       <c r="X665" s="4"/>
       <c r="Y665" s="4"/>
@@ -34278,7 +34832,9 @@
       <c r="AB665" s="4"/>
       <c r="AC665" s="4"/>
       <c r="AD665" s="4"/>
-      <c r="AE665" s="4"/>
+      <c r="AE665" s="4">
+        <v>1</v>
+      </c>
       <c r="AF665" s="4"/>
       <c r="AG665" s="4"/>
       <c r="AH665" s="4"/>
@@ -34387,7 +34943,9 @@
       <c r="K669" s="4"/>
       <c r="L669" s="4"/>
       <c r="M669" s="4"/>
-      <c r="N669" s="4"/>
+      <c r="N669" s="4">
+        <v>7.4999999999999956E-2</v>
+      </c>
       <c r="O669" s="4"/>
       <c r="P669" s="4"/>
       <c r="Q669" s="4"/>
@@ -34513,7 +35071,9 @@
       <c r="K672" s="4"/>
       <c r="L672" s="4"/>
       <c r="M672" s="4"/>
-      <c r="N672" s="4"/>
+      <c r="N672" s="4">
+        <v>7.4999999999999956E-2</v>
+      </c>
       <c r="O672" s="4"/>
       <c r="P672" s="4"/>
       <c r="Q672" s="4"/>
@@ -34639,7 +35199,9 @@
       <c r="K675" s="4"/>
       <c r="L675" s="4"/>
       <c r="M675" s="4"/>
-      <c r="N675" s="4"/>
+      <c r="N675" s="4">
+        <v>6.2E-2</v>
+      </c>
       <c r="O675" s="4"/>
       <c r="P675" s="4"/>
       <c r="Q675" s="4"/>
@@ -34765,7 +35327,9 @@
       <c r="K678" s="4"/>
       <c r="L678" s="4"/>
       <c r="M678" s="4"/>
-      <c r="N678" s="4"/>
+      <c r="N678" s="4">
+        <v>6.2E-2</v>
+      </c>
       <c r="O678" s="4"/>
       <c r="P678" s="4"/>
       <c r="Q678" s="4"/>
@@ -34899,7 +35463,9 @@
       <c r="S681" s="4"/>
       <c r="T681" s="4"/>
       <c r="U681" s="4"/>
-      <c r="V681" s="4"/>
+      <c r="V681" s="4">
+        <v>7.4999999999999956E-2</v>
+      </c>
       <c r="W681" s="4"/>
       <c r="X681" s="4"/>
       <c r="Y681" s="4"/>
@@ -35025,7 +35591,9 @@
       <c r="S684" s="4"/>
       <c r="T684" s="4"/>
       <c r="U684" s="4"/>
-      <c r="V684" s="4"/>
+      <c r="V684" s="4">
+        <v>7.4999999999999956E-2</v>
+      </c>
       <c r="W684" s="4"/>
       <c r="X684" s="4"/>
       <c r="Y684" s="4"/>
@@ -35143,7 +35711,9 @@
       <c r="K687" s="4"/>
       <c r="L687" s="4"/>
       <c r="M687" s="4"/>
-      <c r="N687" s="4"/>
+      <c r="N687" s="4">
+        <v>6.2E-2</v>
+      </c>
       <c r="O687" s="4"/>
       <c r="P687" s="4"/>
       <c r="Q687" s="4"/>
@@ -35157,7 +35727,9 @@
       <c r="Y687" s="4"/>
       <c r="Z687" s="4"/>
       <c r="AA687" s="4"/>
-      <c r="AB687" s="4"/>
+      <c r="AB687" s="4">
+        <v>0.04</v>
+      </c>
       <c r="AC687" s="4"/>
       <c r="AD687" s="4"/>
       <c r="AE687" s="4"/>
@@ -35277,13 +35849,17 @@
       <c r="S690" s="4"/>
       <c r="T690" s="4"/>
       <c r="U690" s="4"/>
-      <c r="V690" s="4"/>
+      <c r="V690" s="4">
+        <v>7.4999999999999956E-2</v>
+      </c>
       <c r="W690" s="4"/>
       <c r="X690" s="4"/>
       <c r="Y690" s="4"/>
       <c r="Z690" s="4"/>
       <c r="AA690" s="4"/>
-      <c r="AB690" s="4"/>
+      <c r="AB690" s="4">
+        <v>0.04</v>
+      </c>
       <c r="AC690" s="4"/>
       <c r="AD690" s="4"/>
       <c r="AE690" s="4"/>
@@ -35647,7 +36223,9 @@
       <c r="K699" s="4"/>
       <c r="L699" s="4"/>
       <c r="M699" s="4"/>
-      <c r="N699" s="4"/>
+      <c r="N699" s="4">
+        <v>6.2E-2</v>
+      </c>
       <c r="O699" s="4"/>
       <c r="P699" s="4"/>
       <c r="Q699" s="4"/>
@@ -35664,7 +36242,9 @@
       <c r="AB699" s="4"/>
       <c r="AC699" s="4"/>
       <c r="AD699" s="4"/>
-      <c r="AE699" s="4"/>
+      <c r="AE699" s="4">
+        <v>1</v>
+      </c>
       <c r="AF699" s="4"/>
       <c r="AG699" s="4"/>
       <c r="AH699" s="4"/>
@@ -35781,7 +36361,9 @@
       <c r="S702" s="4"/>
       <c r="T702" s="4"/>
       <c r="U702" s="4"/>
-      <c r="V702" s="4"/>
+      <c r="V702" s="4">
+        <v>7.4999999999999956E-2</v>
+      </c>
       <c r="W702" s="4"/>
       <c r="X702" s="4"/>
       <c r="Y702" s="4"/>
@@ -35790,7 +36372,9 @@
       <c r="AB702" s="4"/>
       <c r="AC702" s="4"/>
       <c r="AD702" s="4"/>
-      <c r="AE702" s="4"/>
+      <c r="AE702" s="4">
+        <v>1</v>
+      </c>
       <c r="AF702" s="4"/>
       <c r="AG702" s="4"/>
       <c r="AH702" s="4"/>
@@ -35899,7 +36483,9 @@
       <c r="K706" s="4"/>
       <c r="L706" s="4"/>
       <c r="M706" s="4"/>
-      <c r="N706" s="4"/>
+      <c r="N706" s="4">
+        <v>0.95673599999999992</v>
+      </c>
       <c r="O706" s="4"/>
       <c r="P706" s="4"/>
       <c r="Q706" s="4"/>
@@ -36025,7 +36611,9 @@
       <c r="K709" s="4"/>
       <c r="L709" s="4"/>
       <c r="M709" s="4"/>
-      <c r="N709" s="4"/>
+      <c r="N709" s="4">
+        <v>0.95673599999999992</v>
+      </c>
       <c r="O709" s="4"/>
       <c r="P709" s="4"/>
       <c r="Q709" s="4"/>
@@ -36151,7 +36739,9 @@
       <c r="K712" s="4"/>
       <c r="L712" s="4"/>
       <c r="M712" s="4"/>
-      <c r="N712" s="4"/>
+      <c r="N712" s="4">
+        <v>0.95673599999999992</v>
+      </c>
       <c r="O712" s="4"/>
       <c r="P712" s="4"/>
       <c r="Q712" s="4"/>
@@ -36277,7 +36867,9 @@
       <c r="K715" s="4"/>
       <c r="L715" s="4"/>
       <c r="M715" s="4"/>
-      <c r="N715" s="4"/>
+      <c r="N715" s="4">
+        <v>0.95673599999999992</v>
+      </c>
       <c r="O715" s="4"/>
       <c r="P715" s="4"/>
       <c r="Q715" s="4"/>
@@ -36411,7 +37003,9 @@
       <c r="S718" s="4"/>
       <c r="T718" s="4"/>
       <c r="U718" s="4"/>
-      <c r="V718" s="4"/>
+      <c r="V718" s="4">
+        <v>0.95247599999999999</v>
+      </c>
       <c r="W718" s="4"/>
       <c r="X718" s="4"/>
       <c r="Y718" s="4"/>
@@ -36537,7 +37131,9 @@
       <c r="S721" s="4"/>
       <c r="T721" s="4"/>
       <c r="U721" s="4"/>
-      <c r="V721" s="4"/>
+      <c r="V721" s="4">
+        <v>0.95247599999999999</v>
+      </c>
       <c r="W721" s="4"/>
       <c r="X721" s="4"/>
       <c r="Y721" s="4"/>
@@ -36655,7 +37251,9 @@
       <c r="K724" s="4"/>
       <c r="L724" s="4"/>
       <c r="M724" s="4"/>
-      <c r="N724" s="4"/>
+      <c r="N724" s="4">
+        <v>0.95673599999999992</v>
+      </c>
       <c r="O724" s="4"/>
       <c r="P724" s="4"/>
       <c r="Q724" s="4"/>
@@ -36669,7 +37267,9 @@
       <c r="Y724" s="4"/>
       <c r="Z724" s="4"/>
       <c r="AA724" s="4"/>
-      <c r="AB724" s="4"/>
+      <c r="AB724" s="4">
+        <v>0.99839999999999995</v>
+      </c>
       <c r="AC724" s="4"/>
       <c r="AD724" s="4"/>
       <c r="AE724" s="4"/>
@@ -36789,13 +37389,17 @@
       <c r="S727" s="4"/>
       <c r="T727" s="4"/>
       <c r="U727" s="4"/>
-      <c r="V727" s="4"/>
+      <c r="V727" s="4">
+        <v>0.95247599999999999</v>
+      </c>
       <c r="W727" s="4"/>
       <c r="X727" s="4"/>
       <c r="Y727" s="4"/>
       <c r="Z727" s="4"/>
       <c r="AA727" s="4"/>
-      <c r="AB727" s="4"/>
+      <c r="AB727" s="4">
+        <v>0.99839999999999995</v>
+      </c>
       <c r="AC727" s="4"/>
       <c r="AD727" s="4"/>
       <c r="AE727" s="4"/>
@@ -37159,7 +37763,9 @@
       <c r="K736" s="4"/>
       <c r="L736" s="4"/>
       <c r="M736" s="4"/>
-      <c r="N736" s="4"/>
+      <c r="N736" s="4">
+        <v>0.95673599999999992</v>
+      </c>
       <c r="O736" s="4"/>
       <c r="P736" s="4"/>
       <c r="Q736" s="4"/>
@@ -37176,7 +37782,9 @@
       <c r="AB736" s="4"/>
       <c r="AC736" s="4"/>
       <c r="AD736" s="4"/>
-      <c r="AE736" s="4"/>
+      <c r="AE736" s="4">
+        <v>1</v>
+      </c>
       <c r="AF736" s="4"/>
       <c r="AG736" s="4"/>
       <c r="AH736" s="4"/>
@@ -37293,7 +37901,9 @@
       <c r="S739" s="4"/>
       <c r="T739" s="4"/>
       <c r="U739" s="4"/>
-      <c r="V739" s="4"/>
+      <c r="V739" s="4">
+        <v>0.95247599999999999</v>
+      </c>
       <c r="W739" s="4"/>
       <c r="X739" s="4"/>
       <c r="Y739" s="4"/>
@@ -37302,7 +37912,9 @@
       <c r="AB739" s="4"/>
       <c r="AC739" s="4"/>
       <c r="AD739" s="4"/>
-      <c r="AE739" s="4"/>
+      <c r="AE739" s="4">
+        <v>1</v>
+      </c>
       <c r="AF739" s="4"/>
       <c r="AG739" s="4"/>
       <c r="AH739" s="4"/>
@@ -39006,11 +39618,21 @@
       <c r="L780" s="4"/>
       <c r="M780" s="4"/>
       <c r="N780" s="4"/>
-      <c r="O780" s="4"/>
-      <c r="P780" s="4"/>
-      <c r="Q780" s="4"/>
-      <c r="R780" s="4"/>
-      <c r="S780" s="4"/>
+      <c r="O780" s="4">
+        <v>1</v>
+      </c>
+      <c r="P780" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q780" s="4">
+        <v>1</v>
+      </c>
+      <c r="R780" s="4">
+        <v>1</v>
+      </c>
+      <c r="S780" s="4">
+        <v>1</v>
+      </c>
       <c r="T780" s="4"/>
       <c r="U780" s="4"/>
       <c r="V780" s="4"/>
@@ -39132,11 +39754,21 @@
       <c r="L783" s="4"/>
       <c r="M783" s="4"/>
       <c r="N783" s="4"/>
-      <c r="O783" s="4"/>
-      <c r="P783" s="4"/>
-      <c r="Q783" s="4"/>
-      <c r="R783" s="4"/>
-      <c r="S783" s="4"/>
+      <c r="O783" s="4">
+        <v>1</v>
+      </c>
+      <c r="P783" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q783" s="4">
+        <v>1</v>
+      </c>
+      <c r="R783" s="4">
+        <v>1</v>
+      </c>
+      <c r="S783" s="4">
+        <v>1</v>
+      </c>
       <c r="T783" s="4"/>
       <c r="U783" s="4"/>
       <c r="V783" s="4"/>
@@ -39258,11 +39890,21 @@
       <c r="L786" s="4"/>
       <c r="M786" s="4"/>
       <c r="N786" s="4"/>
-      <c r="O786" s="4"/>
-      <c r="P786" s="4"/>
-      <c r="Q786" s="4"/>
-      <c r="R786" s="4"/>
-      <c r="S786" s="4"/>
+      <c r="O786" s="4">
+        <v>1</v>
+      </c>
+      <c r="P786" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q786" s="4">
+        <v>1</v>
+      </c>
+      <c r="R786" s="4">
+        <v>1</v>
+      </c>
+      <c r="S786" s="4">
+        <v>1</v>
+      </c>
       <c r="T786" s="4"/>
       <c r="U786" s="4"/>
       <c r="V786" s="4"/>
@@ -39384,11 +40026,21 @@
       <c r="L789" s="4"/>
       <c r="M789" s="4"/>
       <c r="N789" s="4"/>
-      <c r="O789" s="4"/>
-      <c r="P789" s="4"/>
-      <c r="Q789" s="4"/>
-      <c r="R789" s="4"/>
-      <c r="S789" s="4"/>
+      <c r="O789" s="4">
+        <v>1</v>
+      </c>
+      <c r="P789" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q789" s="4">
+        <v>1</v>
+      </c>
+      <c r="R789" s="4">
+        <v>1</v>
+      </c>
+      <c r="S789" s="4">
+        <v>1</v>
+      </c>
       <c r="T789" s="4"/>
       <c r="U789" s="4"/>
       <c r="V789" s="4"/>
@@ -39518,9 +40170,15 @@
       <c r="T792" s="4"/>
       <c r="U792" s="4"/>
       <c r="V792" s="4"/>
-      <c r="W792" s="4"/>
-      <c r="X792" s="4"/>
-      <c r="Y792" s="4"/>
+      <c r="W792" s="4">
+        <v>1</v>
+      </c>
+      <c r="X792" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y792" s="4">
+        <v>1</v>
+      </c>
       <c r="Z792" s="4"/>
       <c r="AA792" s="4"/>
       <c r="AB792" s="4"/>
@@ -39644,9 +40302,15 @@
       <c r="T795" s="4"/>
       <c r="U795" s="4"/>
       <c r="V795" s="4"/>
-      <c r="W795" s="4"/>
-      <c r="X795" s="4"/>
-      <c r="Y795" s="4"/>
+      <c r="W795" s="4">
+        <v>1</v>
+      </c>
+      <c r="X795" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y795" s="4">
+        <v>1</v>
+      </c>
       <c r="Z795" s="4"/>
       <c r="AA795" s="4"/>
       <c r="AB795" s="4"/>
@@ -39762,11 +40426,21 @@
       <c r="L798" s="4"/>
       <c r="M798" s="4"/>
       <c r="N798" s="4"/>
-      <c r="O798" s="4"/>
-      <c r="P798" s="4"/>
-      <c r="Q798" s="4"/>
-      <c r="R798" s="4"/>
-      <c r="S798" s="4"/>
+      <c r="O798" s="4">
+        <v>1</v>
+      </c>
+      <c r="P798" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q798" s="4">
+        <v>1</v>
+      </c>
+      <c r="R798" s="4">
+        <v>1</v>
+      </c>
+      <c r="S798" s="4">
+        <v>1</v>
+      </c>
       <c r="T798" s="4"/>
       <c r="U798" s="4"/>
       <c r="V798" s="4"/>
@@ -39776,7 +40450,9 @@
       <c r="Z798" s="4"/>
       <c r="AA798" s="4"/>
       <c r="AB798" s="4"/>
-      <c r="AC798" s="4"/>
+      <c r="AC798" s="4">
+        <v>1</v>
+      </c>
       <c r="AD798" s="4"/>
       <c r="AE798" s="4"/>
       <c r="AF798" s="4"/>
@@ -39896,13 +40572,21 @@
       <c r="T801" s="4"/>
       <c r="U801" s="4"/>
       <c r="V801" s="4"/>
-      <c r="W801" s="4"/>
-      <c r="X801" s="4"/>
-      <c r="Y801" s="4"/>
+      <c r="W801" s="4">
+        <v>1</v>
+      </c>
+      <c r="X801" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y801" s="4">
+        <v>1</v>
+      </c>
       <c r="Z801" s="4"/>
       <c r="AA801" s="4"/>
       <c r="AB801" s="4"/>
-      <c r="AC801" s="4"/>
+      <c r="AC801" s="4">
+        <v>1</v>
+      </c>
       <c r="AD801" s="4"/>
       <c r="AE801" s="4"/>
       <c r="AF801" s="4"/>
@@ -40266,11 +40950,21 @@
       <c r="L810" s="4"/>
       <c r="M810" s="4"/>
       <c r="N810" s="4"/>
-      <c r="O810" s="4"/>
-      <c r="P810" s="4"/>
-      <c r="Q810" s="4"/>
-      <c r="R810" s="4"/>
-      <c r="S810" s="4"/>
+      <c r="O810" s="4">
+        <v>1</v>
+      </c>
+      <c r="P810" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q810" s="4">
+        <v>1</v>
+      </c>
+      <c r="R810" s="4">
+        <v>1</v>
+      </c>
+      <c r="S810" s="4">
+        <v>1</v>
+      </c>
       <c r="T810" s="4"/>
       <c r="U810" s="4"/>
       <c r="V810" s="4"/>
@@ -40283,7 +40977,9 @@
       <c r="AC810" s="4"/>
       <c r="AD810" s="4"/>
       <c r="AE810" s="4"/>
-      <c r="AF810" s="4"/>
+      <c r="AF810" s="4">
+        <v>1</v>
+      </c>
       <c r="AG810" s="4"/>
       <c r="AH810" s="4"/>
       <c r="AI810" s="4"/>
@@ -40400,16 +41096,24 @@
       <c r="T813" s="4"/>
       <c r="U813" s="4"/>
       <c r="V813" s="4"/>
-      <c r="W813" s="4"/>
-      <c r="X813" s="4"/>
-      <c r="Y813" s="4"/>
+      <c r="W813" s="4">
+        <v>1</v>
+      </c>
+      <c r="X813" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y813" s="4">
+        <v>1</v>
+      </c>
       <c r="Z813" s="4"/>
       <c r="AA813" s="4"/>
       <c r="AB813" s="4"/>
       <c r="AC813" s="4"/>
       <c r="AD813" s="4"/>
       <c r="AE813" s="4"/>
-      <c r="AF813" s="4"/>
+      <c r="AF813" s="4">
+        <v>1</v>
+      </c>
       <c r="AG813" s="4"/>
       <c r="AH813" s="4"/>
       <c r="AI813" s="4"/>
@@ -40518,11 +41222,21 @@
       <c r="L817" s="4"/>
       <c r="M817" s="4"/>
       <c r="N817" s="4"/>
-      <c r="O817" s="4"/>
-      <c r="P817" s="4"/>
-      <c r="Q817" s="4"/>
-      <c r="R817" s="4"/>
-      <c r="S817" s="4"/>
+      <c r="O817" s="4">
+        <v>0.5524</v>
+      </c>
+      <c r="P817" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Q817" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="R817" s="4">
+        <v>0.31180000000000008</v>
+      </c>
+      <c r="S817" s="4">
+        <v>0.28720000000000001</v>
+      </c>
       <c r="T817" s="4"/>
       <c r="U817" s="4"/>
       <c r="V817" s="4"/>
@@ -40644,11 +41358,21 @@
       <c r="L820" s="4"/>
       <c r="M820" s="4"/>
       <c r="N820" s="4"/>
-      <c r="O820" s="4"/>
-      <c r="P820" s="4"/>
-      <c r="Q820" s="4"/>
-      <c r="R820" s="4"/>
-      <c r="S820" s="4"/>
+      <c r="O820" s="4">
+        <v>0.5524</v>
+      </c>
+      <c r="P820" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Q820" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="R820" s="4">
+        <v>0.31180000000000008</v>
+      </c>
+      <c r="S820" s="4">
+        <v>0.28720000000000001</v>
+      </c>
       <c r="T820" s="4"/>
       <c r="U820" s="4"/>
       <c r="V820" s="4"/>
@@ -40770,11 +41494,21 @@
       <c r="L823" s="4"/>
       <c r="M823" s="4"/>
       <c r="N823" s="4"/>
-      <c r="O823" s="4"/>
-      <c r="P823" s="4"/>
-      <c r="Q823" s="4"/>
-      <c r="R823" s="4"/>
-      <c r="S823" s="4"/>
+      <c r="O823" s="4">
+        <v>0.5524</v>
+      </c>
+      <c r="P823" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Q823" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="R823" s="4">
+        <v>0.31180000000000008</v>
+      </c>
+      <c r="S823" s="4">
+        <v>0.28720000000000001</v>
+      </c>
       <c r="T823" s="4"/>
       <c r="U823" s="4"/>
       <c r="V823" s="4"/>
@@ -40896,11 +41630,21 @@
       <c r="L826" s="4"/>
       <c r="M826" s="4"/>
       <c r="N826" s="4"/>
-      <c r="O826" s="4"/>
-      <c r="P826" s="4"/>
-      <c r="Q826" s="4"/>
-      <c r="R826" s="4"/>
-      <c r="S826" s="4"/>
+      <c r="O826" s="4">
+        <v>0.5524</v>
+      </c>
+      <c r="P826" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Q826" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="R826" s="4">
+        <v>0.31180000000000008</v>
+      </c>
+      <c r="S826" s="4">
+        <v>0.28720000000000001</v>
+      </c>
       <c r="T826" s="4"/>
       <c r="U826" s="4"/>
       <c r="V826" s="4"/>
@@ -41030,9 +41774,15 @@
       <c r="T829" s="4"/>
       <c r="U829" s="4"/>
       <c r="V829" s="4"/>
-      <c r="W829" s="4"/>
-      <c r="X829" s="4"/>
-      <c r="Y829" s="4"/>
+      <c r="W829" s="4">
+        <v>0.44720000000000004</v>
+      </c>
+      <c r="X829" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Y829" s="4">
+        <v>0.14529999999999998</v>
+      </c>
       <c r="Z829" s="4"/>
       <c r="AA829" s="4"/>
       <c r="AB829" s="4"/>
@@ -41156,9 +41906,15 @@
       <c r="T832" s="4"/>
       <c r="U832" s="4"/>
       <c r="V832" s="4"/>
-      <c r="W832" s="4"/>
-      <c r="X832" s="4"/>
-      <c r="Y832" s="4"/>
+      <c r="W832" s="4">
+        <v>0.44720000000000004</v>
+      </c>
+      <c r="X832" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Y832" s="4">
+        <v>0.14529999999999998</v>
+      </c>
       <c r="Z832" s="4"/>
       <c r="AA832" s="4"/>
       <c r="AB832" s="4"/>
@@ -41274,11 +42030,21 @@
       <c r="L835" s="4"/>
       <c r="M835" s="4"/>
       <c r="N835" s="4"/>
-      <c r="O835" s="4"/>
-      <c r="P835" s="4"/>
-      <c r="Q835" s="4"/>
-      <c r="R835" s="4"/>
-      <c r="S835" s="4"/>
+      <c r="O835" s="4">
+        <v>0.5524</v>
+      </c>
+      <c r="P835" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Q835" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="R835" s="4">
+        <v>0.31180000000000008</v>
+      </c>
+      <c r="S835" s="4">
+        <v>0.28720000000000001</v>
+      </c>
       <c r="T835" s="4"/>
       <c r="U835" s="4"/>
       <c r="V835" s="4"/>
@@ -41288,7 +42054,9 @@
       <c r="Z835" s="4"/>
       <c r="AA835" s="4"/>
       <c r="AB835" s="4"/>
-      <c r="AC835" s="4"/>
+      <c r="AC835" s="4">
+        <v>1</v>
+      </c>
       <c r="AD835" s="4"/>
       <c r="AE835" s="4"/>
       <c r="AF835" s="4"/>
@@ -41408,13 +42176,21 @@
       <c r="T838" s="4"/>
       <c r="U838" s="4"/>
       <c r="V838" s="4"/>
-      <c r="W838" s="4"/>
-      <c r="X838" s="4"/>
-      <c r="Y838" s="4"/>
+      <c r="W838" s="4">
+        <v>0.44720000000000004</v>
+      </c>
+      <c r="X838" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Y838" s="4">
+        <v>0.14529999999999998</v>
+      </c>
       <c r="Z838" s="4"/>
       <c r="AA838" s="4"/>
       <c r="AB838" s="4"/>
-      <c r="AC838" s="4"/>
+      <c r="AC838" s="4">
+        <v>1</v>
+      </c>
       <c r="AD838" s="4"/>
       <c r="AE838" s="4"/>
       <c r="AF838" s="4"/>
@@ -41778,11 +42554,21 @@
       <c r="L847" s="4"/>
       <c r="M847" s="4"/>
       <c r="N847" s="4"/>
-      <c r="O847" s="4"/>
-      <c r="P847" s="4"/>
-      <c r="Q847" s="4"/>
-      <c r="R847" s="4"/>
-      <c r="S847" s="4"/>
+      <c r="O847" s="4">
+        <v>0.5524</v>
+      </c>
+      <c r="P847" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Q847" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="R847" s="4">
+        <v>0.31180000000000008</v>
+      </c>
+      <c r="S847" s="4">
+        <v>0.28720000000000001</v>
+      </c>
       <c r="T847" s="4"/>
       <c r="U847" s="4"/>
       <c r="V847" s="4"/>
@@ -41795,7 +42581,9 @@
       <c r="AC847" s="4"/>
       <c r="AD847" s="4"/>
       <c r="AE847" s="4"/>
-      <c r="AF847" s="4"/>
+      <c r="AF847" s="4">
+        <v>1</v>
+      </c>
       <c r="AG847" s="4"/>
       <c r="AH847" s="4"/>
       <c r="AI847" s="4"/>
@@ -41912,16 +42700,24 @@
       <c r="T850" s="4"/>
       <c r="U850" s="4"/>
       <c r="V850" s="4"/>
-      <c r="W850" s="4"/>
-      <c r="X850" s="4"/>
-      <c r="Y850" s="4"/>
+      <c r="W850" s="4">
+        <v>0.44720000000000004</v>
+      </c>
+      <c r="X850" s="4">
+        <v>0.28720000000000001</v>
+      </c>
+      <c r="Y850" s="4">
+        <v>0.14529999999999998</v>
+      </c>
       <c r="Z850" s="4"/>
       <c r="AA850" s="4"/>
       <c r="AB850" s="4"/>
       <c r="AC850" s="4"/>
       <c r="AD850" s="4"/>
       <c r="AE850" s="4"/>
-      <c r="AF850" s="4"/>
+      <c r="AF850" s="4">
+        <v>1</v>
+      </c>
       <c r="AG850" s="4"/>
       <c r="AH850" s="4"/>
       <c r="AI850" s="4"/>
@@ -42030,11 +42826,21 @@
       <c r="L854" s="4"/>
       <c r="M854" s="4"/>
       <c r="N854" s="4"/>
-      <c r="O854" s="4"/>
-      <c r="P854" s="4"/>
-      <c r="Q854" s="4"/>
-      <c r="R854" s="4"/>
-      <c r="S854" s="4"/>
+      <c r="O854" s="4">
+        <v>0.39816945906675694</v>
+      </c>
+      <c r="P854" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Q854" s="4">
+        <v>0.52714374529406949</v>
+      </c>
+      <c r="R854" s="4">
+        <v>0.68592239052443116</v>
+      </c>
+      <c r="S854" s="4">
+        <v>0.74456761445968844</v>
+      </c>
       <c r="T854" s="4"/>
       <c r="U854" s="4"/>
       <c r="V854" s="4"/>
@@ -42156,11 +42962,21 @@
       <c r="L857" s="4"/>
       <c r="M857" s="4"/>
       <c r="N857" s="4"/>
-      <c r="O857" s="4"/>
-      <c r="P857" s="4"/>
-      <c r="Q857" s="4"/>
-      <c r="R857" s="4"/>
-      <c r="S857" s="4"/>
+      <c r="O857" s="4">
+        <v>0.39816945906675694</v>
+      </c>
+      <c r="P857" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Q857" s="4">
+        <v>0.52714374529406949</v>
+      </c>
+      <c r="R857" s="4">
+        <v>0.68592239052443116</v>
+      </c>
+      <c r="S857" s="4">
+        <v>0.74456761445968844</v>
+      </c>
       <c r="T857" s="4"/>
       <c r="U857" s="4"/>
       <c r="V857" s="4"/>
@@ -42282,11 +43098,21 @@
       <c r="L860" s="4"/>
       <c r="M860" s="4"/>
       <c r="N860" s="4"/>
-      <c r="O860" s="4"/>
-      <c r="P860" s="4"/>
-      <c r="Q860" s="4"/>
-      <c r="R860" s="4"/>
-      <c r="S860" s="4"/>
+      <c r="O860" s="4">
+        <v>0.39816945906675694</v>
+      </c>
+      <c r="P860" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Q860" s="4">
+        <v>0.52714374529406949</v>
+      </c>
+      <c r="R860" s="4">
+        <v>0.68592239052443116</v>
+      </c>
+      <c r="S860" s="4">
+        <v>0.74456761445968844</v>
+      </c>
       <c r="T860" s="4"/>
       <c r="U860" s="4"/>
       <c r="V860" s="4"/>
@@ -42408,11 +43234,21 @@
       <c r="L863" s="4"/>
       <c r="M863" s="4"/>
       <c r="N863" s="4"/>
-      <c r="O863" s="4"/>
-      <c r="P863" s="4"/>
-      <c r="Q863" s="4"/>
-      <c r="R863" s="4"/>
-      <c r="S863" s="4"/>
+      <c r="O863" s="4">
+        <v>0.39816945906675694</v>
+      </c>
+      <c r="P863" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Q863" s="4">
+        <v>0.52714374529406949</v>
+      </c>
+      <c r="R863" s="4">
+        <v>0.68592239052443116</v>
+      </c>
+      <c r="S863" s="4">
+        <v>0.74456761445968844</v>
+      </c>
       <c r="T863" s="4"/>
       <c r="U863" s="4"/>
       <c r="V863" s="4"/>
@@ -42542,9 +43378,15 @@
       <c r="T866" s="4"/>
       <c r="U866" s="4"/>
       <c r="V866" s="4"/>
-      <c r="W866" s="4"/>
-      <c r="X866" s="4"/>
-      <c r="Y866" s="4"/>
+      <c r="W866" s="4">
+        <v>0.33411712741654032</v>
+      </c>
+      <c r="X866" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Y866" s="4">
+        <v>0.61708679020377177</v>
+      </c>
       <c r="Z866" s="4"/>
       <c r="AA866" s="4"/>
       <c r="AB866" s="4"/>
@@ -42668,9 +43510,15 @@
       <c r="T869" s="4"/>
       <c r="U869" s="4"/>
       <c r="V869" s="4"/>
-      <c r="W869" s="4"/>
-      <c r="X869" s="4"/>
-      <c r="Y869" s="4"/>
+      <c r="W869" s="4">
+        <v>0.33411712741654032</v>
+      </c>
+      <c r="X869" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Y869" s="4">
+        <v>0.61708679020377177</v>
+      </c>
       <c r="Z869" s="4"/>
       <c r="AA869" s="4"/>
       <c r="AB869" s="4"/>
@@ -42786,11 +43634,21 @@
       <c r="L872" s="4"/>
       <c r="M872" s="4"/>
       <c r="N872" s="4"/>
-      <c r="O872" s="4"/>
-      <c r="P872" s="4"/>
-      <c r="Q872" s="4"/>
-      <c r="R872" s="4"/>
-      <c r="S872" s="4"/>
+      <c r="O872" s="4">
+        <v>0.39816945906675694</v>
+      </c>
+      <c r="P872" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Q872" s="4">
+        <v>0.52714374529406949</v>
+      </c>
+      <c r="R872" s="4">
+        <v>0.68592239052443116</v>
+      </c>
+      <c r="S872" s="4">
+        <v>0.74456761445968844</v>
+      </c>
       <c r="T872" s="4"/>
       <c r="U872" s="4"/>
       <c r="V872" s="4"/>
@@ -42800,7 +43658,9 @@
       <c r="Z872" s="4"/>
       <c r="AA872" s="4"/>
       <c r="AB872" s="4"/>
-      <c r="AC872" s="4"/>
+      <c r="AC872" s="4">
+        <v>0</v>
+      </c>
       <c r="AD872" s="4"/>
       <c r="AE872" s="4"/>
       <c r="AF872" s="4"/>
@@ -42920,13 +43780,21 @@
       <c r="T875" s="4"/>
       <c r="U875" s="4"/>
       <c r="V875" s="4"/>
-      <c r="W875" s="4"/>
-      <c r="X875" s="4"/>
-      <c r="Y875" s="4"/>
+      <c r="W875" s="4">
+        <v>0.33411712741654032</v>
+      </c>
+      <c r="X875" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Y875" s="4">
+        <v>0.61708679020377177</v>
+      </c>
       <c r="Z875" s="4"/>
       <c r="AA875" s="4"/>
       <c r="AB875" s="4"/>
-      <c r="AC875" s="4"/>
+      <c r="AC875" s="4">
+        <v>0</v>
+      </c>
       <c r="AD875" s="4"/>
       <c r="AE875" s="4"/>
       <c r="AF875" s="4"/>
@@ -43290,11 +44158,21 @@
       <c r="L884" s="4"/>
       <c r="M884" s="4"/>
       <c r="N884" s="4"/>
-      <c r="O884" s="4"/>
-      <c r="P884" s="4"/>
-      <c r="Q884" s="4"/>
-      <c r="R884" s="4"/>
-      <c r="S884" s="4"/>
+      <c r="O884" s="4">
+        <v>0.39816945906675694</v>
+      </c>
+      <c r="P884" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Q884" s="4">
+        <v>0.52714374529406949</v>
+      </c>
+      <c r="R884" s="4">
+        <v>0.68592239052443116</v>
+      </c>
+      <c r="S884" s="4">
+        <v>0.74456761445968844</v>
+      </c>
       <c r="T884" s="4"/>
       <c r="U884" s="4"/>
       <c r="V884" s="4"/>
@@ -43307,7 +44185,9 @@
       <c r="AC884" s="4"/>
       <c r="AD884" s="4"/>
       <c r="AE884" s="4"/>
-      <c r="AF884" s="4"/>
+      <c r="AF884" s="4">
+        <v>0</v>
+      </c>
       <c r="AG884" s="4"/>
       <c r="AH884" s="4"/>
       <c r="AI884" s="4"/>
@@ -43424,16 +44304,24 @@
       <c r="T887" s="4"/>
       <c r="U887" s="4"/>
       <c r="V887" s="4"/>
-      <c r="W887" s="4"/>
-      <c r="X887" s="4"/>
-      <c r="Y887" s="4"/>
+      <c r="W887" s="4">
+        <v>0.33411712741654032</v>
+      </c>
+      <c r="X887" s="4">
+        <v>0.46427619056084501</v>
+      </c>
+      <c r="Y887" s="4">
+        <v>0.61708679020377177</v>
+      </c>
       <c r="Z887" s="4"/>
       <c r="AA887" s="4"/>
       <c r="AB887" s="4"/>
       <c r="AC887" s="4"/>
       <c r="AD887" s="4"/>
       <c r="AE887" s="4"/>
-      <c r="AF887" s="4"/>
+      <c r="AF887" s="4">
+        <v>0</v>
+      </c>
       <c r="AG887" s="4"/>
       <c r="AH887" s="4"/>
       <c r="AI887" s="4"/>
@@ -45141,8 +46029,12 @@
       <c r="Q928" s="4"/>
       <c r="R928" s="4"/>
       <c r="S928" s="4"/>
-      <c r="T928" s="4"/>
-      <c r="U928" s="4"/>
+      <c r="T928" s="4">
+        <v>1</v>
+      </c>
+      <c r="U928" s="4">
+        <v>1</v>
+      </c>
       <c r="V928" s="4"/>
       <c r="W928" s="4"/>
       <c r="X928" s="4"/>
@@ -45267,8 +46159,12 @@
       <c r="Q931" s="4"/>
       <c r="R931" s="4"/>
       <c r="S931" s="4"/>
-      <c r="T931" s="4"/>
-      <c r="U931" s="4"/>
+      <c r="T931" s="4">
+        <v>1</v>
+      </c>
+      <c r="U931" s="4">
+        <v>1</v>
+      </c>
       <c r="V931" s="4"/>
       <c r="W931" s="4"/>
       <c r="X931" s="4"/>
@@ -45393,8 +46289,12 @@
       <c r="Q934" s="4"/>
       <c r="R934" s="4"/>
       <c r="S934" s="4"/>
-      <c r="T934" s="4"/>
-      <c r="U934" s="4"/>
+      <c r="T934" s="4">
+        <v>1</v>
+      </c>
+      <c r="U934" s="4">
+        <v>1</v>
+      </c>
       <c r="V934" s="4"/>
       <c r="W934" s="4"/>
       <c r="X934" s="4"/>
@@ -45519,8 +46419,12 @@
       <c r="Q937" s="4"/>
       <c r="R937" s="4"/>
       <c r="S937" s="4"/>
-      <c r="T937" s="4"/>
-      <c r="U937" s="4"/>
+      <c r="T937" s="4">
+        <v>1</v>
+      </c>
+      <c r="U937" s="4">
+        <v>1</v>
+      </c>
       <c r="V937" s="4"/>
       <c r="W937" s="4"/>
       <c r="X937" s="4"/>
@@ -45651,8 +46555,12 @@
       <c r="W940" s="4"/>
       <c r="X940" s="4"/>
       <c r="Y940" s="4"/>
-      <c r="Z940" s="4"/>
-      <c r="AA940" s="4"/>
+      <c r="Z940" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA940" s="4">
+        <v>1</v>
+      </c>
       <c r="AB940" s="4"/>
       <c r="AC940" s="4"/>
       <c r="AD940" s="4"/>
@@ -45777,8 +46685,12 @@
       <c r="W943" s="4"/>
       <c r="X943" s="4"/>
       <c r="Y943" s="4"/>
-      <c r="Z943" s="4"/>
-      <c r="AA943" s="4"/>
+      <c r="Z943" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA943" s="4">
+        <v>1</v>
+      </c>
       <c r="AB943" s="4"/>
       <c r="AC943" s="4"/>
       <c r="AD943" s="4"/>
@@ -45897,8 +46809,12 @@
       <c r="Q946" s="4"/>
       <c r="R946" s="4"/>
       <c r="S946" s="4"/>
-      <c r="T946" s="4"/>
-      <c r="U946" s="4"/>
+      <c r="T946" s="4">
+        <v>1</v>
+      </c>
+      <c r="U946" s="4">
+        <v>1</v>
+      </c>
       <c r="V946" s="4"/>
       <c r="W946" s="4"/>
       <c r="X946" s="4"/>
@@ -45907,7 +46823,9 @@
       <c r="AA946" s="4"/>
       <c r="AB946" s="4"/>
       <c r="AC946" s="4"/>
-      <c r="AD946" s="4"/>
+      <c r="AD946" s="4">
+        <v>1</v>
+      </c>
       <c r="AE946" s="4"/>
       <c r="AF946" s="4"/>
       <c r="AG946" s="4"/>
@@ -46029,11 +46947,17 @@
       <c r="W949" s="4"/>
       <c r="X949" s="4"/>
       <c r="Y949" s="4"/>
-      <c r="Z949" s="4"/>
-      <c r="AA949" s="4"/>
+      <c r="Z949" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA949" s="4">
+        <v>1</v>
+      </c>
       <c r="AB949" s="4"/>
       <c r="AC949" s="4"/>
-      <c r="AD949" s="4"/>
+      <c r="AD949" s="4">
+        <v>1</v>
+      </c>
       <c r="AE949" s="4"/>
       <c r="AF949" s="4"/>
       <c r="AG949" s="4"/>
@@ -46401,8 +47325,12 @@
       <c r="Q958" s="4"/>
       <c r="R958" s="4"/>
       <c r="S958" s="4"/>
-      <c r="T958" s="4"/>
-      <c r="U958" s="4"/>
+      <c r="T958" s="4">
+        <v>1</v>
+      </c>
+      <c r="U958" s="4">
+        <v>1</v>
+      </c>
       <c r="V958" s="4"/>
       <c r="W958" s="4"/>
       <c r="X958" s="4"/>
@@ -46414,7 +47342,9 @@
       <c r="AD958" s="4"/>
       <c r="AE958" s="4"/>
       <c r="AF958" s="4"/>
-      <c r="AG958" s="4"/>
+      <c r="AG958" s="4">
+        <v>1</v>
+      </c>
       <c r="AH958" s="4"/>
       <c r="AI958" s="4"/>
       <c r="AJ958" s="4"/>
@@ -46533,14 +47463,20 @@
       <c r="W961" s="4"/>
       <c r="X961" s="4"/>
       <c r="Y961" s="4"/>
-      <c r="Z961" s="4"/>
-      <c r="AA961" s="4"/>
+      <c r="Z961" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA961" s="4">
+        <v>1</v>
+      </c>
       <c r="AB961" s="4"/>
       <c r="AC961" s="4"/>
       <c r="AD961" s="4"/>
       <c r="AE961" s="4"/>
       <c r="AF961" s="4"/>
-      <c r="AG961" s="4"/>
+      <c r="AG961" s="4">
+        <v>1</v>
+      </c>
       <c r="AH961" s="4"/>
       <c r="AI961" s="4"/>
       <c r="AJ961" s="4"/>
@@ -46653,8 +47589,12 @@
       <c r="Q965" s="4"/>
       <c r="R965" s="4"/>
       <c r="S965" s="4"/>
-      <c r="T965" s="4"/>
-      <c r="U965" s="4"/>
+      <c r="T965" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="U965" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="V965" s="4"/>
       <c r="W965" s="4"/>
       <c r="X965" s="4"/>
@@ -46779,8 +47719,12 @@
       <c r="Q968" s="4"/>
       <c r="R968" s="4"/>
       <c r="S968" s="4"/>
-      <c r="T968" s="4"/>
-      <c r="U968" s="4"/>
+      <c r="T968" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="U968" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="V968" s="4"/>
       <c r="W968" s="4"/>
       <c r="X968" s="4"/>
@@ -46905,8 +47849,12 @@
       <c r="Q971" s="4"/>
       <c r="R971" s="4"/>
       <c r="S971" s="4"/>
-      <c r="T971" s="4"/>
-      <c r="U971" s="4"/>
+      <c r="T971" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="U971" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="V971" s="4"/>
       <c r="W971" s="4"/>
       <c r="X971" s="4"/>
@@ -47031,8 +47979,12 @@
       <c r="Q974" s="4"/>
       <c r="R974" s="4"/>
       <c r="S974" s="4"/>
-      <c r="T974" s="4"/>
-      <c r="U974" s="4"/>
+      <c r="T974" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="U974" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="V974" s="4"/>
       <c r="W974" s="4"/>
       <c r="X974" s="4"/>
@@ -47163,8 +48115,12 @@
       <c r="W977" s="4"/>
       <c r="X977" s="4"/>
       <c r="Y977" s="4"/>
-      <c r="Z977" s="4"/>
-      <c r="AA977" s="4"/>
+      <c r="Z977" s="4">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="AA977" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="AB977" s="4"/>
       <c r="AC977" s="4"/>
       <c r="AD977" s="4"/>
@@ -47289,8 +48245,12 @@
       <c r="W980" s="4"/>
       <c r="X980" s="4"/>
       <c r="Y980" s="4"/>
-      <c r="Z980" s="4"/>
-      <c r="AA980" s="4"/>
+      <c r="Z980" s="4">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="AA980" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="AB980" s="4"/>
       <c r="AC980" s="4"/>
       <c r="AD980" s="4"/>
@@ -47409,8 +48369,12 @@
       <c r="Q983" s="4"/>
       <c r="R983" s="4"/>
       <c r="S983" s="4"/>
-      <c r="T983" s="4"/>
-      <c r="U983" s="4"/>
+      <c r="T983" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="U983" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="V983" s="4"/>
       <c r="W983" s="4"/>
       <c r="X983" s="4"/>
@@ -47419,7 +48383,9 @@
       <c r="AA983" s="4"/>
       <c r="AB983" s="4"/>
       <c r="AC983" s="4"/>
-      <c r="AD983" s="4"/>
+      <c r="AD983" s="4">
+        <v>1</v>
+      </c>
       <c r="AE983" s="4"/>
       <c r="AF983" s="4"/>
       <c r="AG983" s="4"/>
@@ -47541,11 +48507,17 @@
       <c r="W986" s="4"/>
       <c r="X986" s="4"/>
       <c r="Y986" s="4"/>
-      <c r="Z986" s="4"/>
-      <c r="AA986" s="4"/>
+      <c r="Z986" s="4">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="AA986" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="AB986" s="4"/>
       <c r="AC986" s="4"/>
-      <c r="AD986" s="4"/>
+      <c r="AD986" s="4">
+        <v>1</v>
+      </c>
       <c r="AE986" s="4"/>
       <c r="AF986" s="4"/>
       <c r="AG986" s="4"/>
@@ -47913,8 +48885,12 @@
       <c r="Q995" s="4"/>
       <c r="R995" s="4"/>
       <c r="S995" s="4"/>
-      <c r="T995" s="4"/>
-      <c r="U995" s="4"/>
+      <c r="T995" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="U995" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="V995" s="4"/>
       <c r="W995" s="4"/>
       <c r="X995" s="4"/>
@@ -47926,7 +48902,9 @@
       <c r="AD995" s="4"/>
       <c r="AE995" s="4"/>
       <c r="AF995" s="4"/>
-      <c r="AG995" s="4"/>
+      <c r="AG995" s="4">
+        <v>1</v>
+      </c>
       <c r="AH995" s="4"/>
       <c r="AI995" s="4"/>
       <c r="AJ995" s="4"/>
@@ -48045,14 +49023,20 @@
       <c r="W998" s="4"/>
       <c r="X998" s="4"/>
       <c r="Y998" s="4"/>
-      <c r="Z998" s="4"/>
-      <c r="AA998" s="4"/>
+      <c r="Z998" s="4">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="AA998" s="4">
+        <v>0.1090000000000001</v>
+      </c>
       <c r="AB998" s="4"/>
       <c r="AC998" s="4"/>
       <c r="AD998" s="4"/>
       <c r="AE998" s="4"/>
       <c r="AF998" s="4"/>
-      <c r="AG998" s="4"/>
+      <c r="AG998" s="4">
+        <v>1</v>
+      </c>
       <c r="AH998" s="4"/>
       <c r="AI998" s="4"/>
       <c r="AJ998" s="4"/>
@@ -48165,8 +49149,12 @@
       <c r="Q1002" s="4"/>
       <c r="R1002" s="4"/>
       <c r="S1002" s="4"/>
-      <c r="T1002" s="4"/>
-      <c r="U1002" s="4"/>
+      <c r="T1002" s="4">
+        <v>0.38926274061590116</v>
+      </c>
+      <c r="U1002" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="V1002" s="4"/>
       <c r="W1002" s="4"/>
       <c r="X1002" s="4"/>
@@ -48291,8 +49279,12 @@
       <c r="Q1005" s="4"/>
       <c r="R1005" s="4"/>
       <c r="S1005" s="4"/>
-      <c r="T1005" s="4"/>
-      <c r="U1005" s="4"/>
+      <c r="T1005" s="4">
+        <v>0.38926274061590116</v>
+      </c>
+      <c r="U1005" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="V1005" s="4"/>
       <c r="W1005" s="4"/>
       <c r="X1005" s="4"/>
@@ -48417,8 +49409,12 @@
       <c r="Q1008" s="4"/>
       <c r="R1008" s="4"/>
       <c r="S1008" s="4"/>
-      <c r="T1008" s="4"/>
-      <c r="U1008" s="4"/>
+      <c r="T1008" s="4">
+        <v>0.38926274061590116</v>
+      </c>
+      <c r="U1008" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="V1008" s="4"/>
       <c r="W1008" s="4"/>
       <c r="X1008" s="4"/>
@@ -48543,8 +49539,12 @@
       <c r="Q1011" s="4"/>
       <c r="R1011" s="4"/>
       <c r="S1011" s="4"/>
-      <c r="T1011" s="4"/>
-      <c r="U1011" s="4"/>
+      <c r="T1011" s="4">
+        <v>0.38926274061590116</v>
+      </c>
+      <c r="U1011" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="V1011" s="4"/>
       <c r="W1011" s="4"/>
       <c r="X1011" s="4"/>
@@ -48675,8 +49675,12 @@
       <c r="W1014" s="4"/>
       <c r="X1014" s="4"/>
       <c r="Y1014" s="4"/>
-      <c r="Z1014" s="4"/>
-      <c r="AA1014" s="4"/>
+      <c r="Z1014" s="4">
+        <v>0.2344936316398144</v>
+      </c>
+      <c r="AA1014" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="AB1014" s="4"/>
       <c r="AC1014" s="4"/>
       <c r="AD1014" s="4"/>
@@ -48801,8 +49805,12 @@
       <c r="W1017" s="4"/>
       <c r="X1017" s="4"/>
       <c r="Y1017" s="4"/>
-      <c r="Z1017" s="4"/>
-      <c r="AA1017" s="4"/>
+      <c r="Z1017" s="4">
+        <v>0.2344936316398144</v>
+      </c>
+      <c r="AA1017" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="AB1017" s="4"/>
       <c r="AC1017" s="4"/>
       <c r="AD1017" s="4"/>
@@ -48921,8 +49929,12 @@
       <c r="Q1020" s="4"/>
       <c r="R1020" s="4"/>
       <c r="S1020" s="4"/>
-      <c r="T1020" s="4"/>
-      <c r="U1020" s="4"/>
+      <c r="T1020" s="4">
+        <v>0.38926274061590116</v>
+      </c>
+      <c r="U1020" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="V1020" s="4"/>
       <c r="W1020" s="4"/>
       <c r="X1020" s="4"/>
@@ -48931,7 +49943,9 @@
       <c r="AA1020" s="4"/>
       <c r="AB1020" s="4"/>
       <c r="AC1020" s="4"/>
-      <c r="AD1020" s="4"/>
+      <c r="AD1020" s="4">
+        <v>0</v>
+      </c>
       <c r="AE1020" s="4"/>
       <c r="AF1020" s="4"/>
       <c r="AG1020" s="4"/>
@@ -49053,11 +50067,17 @@
       <c r="W1023" s="4"/>
       <c r="X1023" s="4"/>
       <c r="Y1023" s="4"/>
-      <c r="Z1023" s="4"/>
-      <c r="AA1023" s="4"/>
+      <c r="Z1023" s="4">
+        <v>0.2344936316398144</v>
+      </c>
+      <c r="AA1023" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="AB1023" s="4"/>
       <c r="AC1023" s="4"/>
-      <c r="AD1023" s="4"/>
+      <c r="AD1023" s="4">
+        <v>0</v>
+      </c>
       <c r="AE1023" s="4"/>
       <c r="AF1023" s="4"/>
       <c r="AG1023" s="4"/>
@@ -49425,8 +50445,12 @@
       <c r="Q1032" s="4"/>
       <c r="R1032" s="4"/>
       <c r="S1032" s="4"/>
-      <c r="T1032" s="4"/>
-      <c r="U1032" s="4"/>
+      <c r="T1032" s="4">
+        <v>0.38926274061590116</v>
+      </c>
+      <c r="U1032" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="V1032" s="4"/>
       <c r="W1032" s="4"/>
       <c r="X1032" s="4"/>
@@ -49438,7 +50462,9 @@
       <c r="AD1032" s="4"/>
       <c r="AE1032" s="4"/>
       <c r="AF1032" s="4"/>
-      <c r="AG1032" s="4"/>
+      <c r="AG1032" s="4">
+        <v>0</v>
+      </c>
       <c r="AH1032" s="4"/>
       <c r="AI1032" s="4"/>
       <c r="AJ1032" s="4"/>
@@ -49557,14 +50583,20 @@
       <c r="W1035" s="4"/>
       <c r="X1035" s="4"/>
       <c r="Y1035" s="4"/>
-      <c r="Z1035" s="4"/>
-      <c r="AA1035" s="4"/>
+      <c r="Z1035" s="4">
+        <v>0.2344936316398144</v>
+      </c>
+      <c r="AA1035" s="4">
+        <v>0.46333193430953246</v>
+      </c>
       <c r="AB1035" s="4"/>
       <c r="AC1035" s="4"/>
       <c r="AD1035" s="4"/>
       <c r="AE1035" s="4"/>
       <c r="AF1035" s="4"/>
-      <c r="AG1035" s="4"/>
+      <c r="AG1035" s="4">
+        <v>0</v>
+      </c>
       <c r="AH1035" s="4"/>
       <c r="AI1035" s="4"/>
       <c r="AJ1035" s="4"/>

</xml_diff>

<commit_message>
temp remove max val
</commit_message>
<xml_diff>
--- a/tests/databooks/progbook_tb.xlsx
+++ b/tests/databooks/progbook_tb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/databooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{24FB7F02-D6E9-9643-B118-B24414A4C0AD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4EC83AF3-59D0-DF40-8108-3641F6C509DC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="26160" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -543,9 +543,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -911,10 +908,10 @@
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="F1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="S1" s="8" t="s">
+      <c r="F1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1052,10 +1049,10 @@
       <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>79</v>
       </c>
       <c r="E3" s="3"/>
@@ -1110,10 +1107,10 @@
       <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>81</v>
       </c>
       <c r="E4" s="3"/>
@@ -1188,10 +1185,10 @@
       <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>83</v>
       </c>
       <c r="E5" s="3"/>
@@ -1266,10 +1263,10 @@
       <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E6" s="3"/>
@@ -1344,10 +1341,10 @@
       <c r="B7" s="4">
         <v>5</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>87</v>
       </c>
       <c r="E7" s="3"/>
@@ -1422,10 +1419,10 @@
       <c r="B8" s="4">
         <v>6</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>89</v>
       </c>
       <c r="E8" s="3"/>
@@ -1504,10 +1501,10 @@
       <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>91</v>
       </c>
       <c r="E9" s="3"/>
@@ -1578,10 +1575,10 @@
       <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>93</v>
       </c>
       <c r="E10" s="3"/>
@@ -1648,10 +1645,10 @@
       <c r="B11" s="4">
         <v>9</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>95</v>
       </c>
       <c r="E11" s="3"/>
@@ -1718,10 +1715,10 @@
       <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>97</v>
       </c>
       <c r="E12" s="3"/>
@@ -1788,10 +1785,10 @@
       <c r="B13" s="4">
         <v>11</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>99</v>
       </c>
       <c r="E13" s="3"/>
@@ -1858,10 +1855,10 @@
       <c r="B14" s="4">
         <v>12</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>101</v>
       </c>
       <c r="E14" s="3"/>
@@ -1928,10 +1925,10 @@
       <c r="B15" s="4">
         <v>13</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>103</v>
       </c>
       <c r="E15" s="3"/>
@@ -1998,10 +1995,10 @@
       <c r="B16" s="4">
         <v>14</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>105</v>
       </c>
       <c r="E16" s="3"/>
@@ -2068,10 +2065,10 @@
       <c r="B17" s="4">
         <v>15</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>107</v>
       </c>
       <c r="E17" s="3"/>
@@ -2138,10 +2135,10 @@
       <c r="B18" s="4">
         <v>16</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>109</v>
       </c>
       <c r="E18" s="3"/>
@@ -2204,10 +2201,10 @@
       <c r="B19" s="4">
         <v>17</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>111</v>
       </c>
       <c r="E19" s="3"/>
@@ -2270,10 +2267,10 @@
       <c r="B20" s="4">
         <v>18</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>113</v>
       </c>
       <c r="E20" s="3"/>
@@ -2336,10 +2333,10 @@
       <c r="B21" s="4">
         <v>19</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>115</v>
       </c>
       <c r="E21" s="3"/>
@@ -2402,10 +2399,10 @@
       <c r="B22" s="4">
         <v>20</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E22" s="3"/>
@@ -2468,10 +2465,10 @@
       <c r="B23" s="4">
         <v>21</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>119</v>
       </c>
       <c r="E23" s="3"/>
@@ -2534,10 +2531,10 @@
       <c r="B24" s="4">
         <v>22</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="11" t="s">
         <v>121</v>
       </c>
       <c r="E24" s="3"/>
@@ -2592,10 +2589,10 @@
       <c r="B25" s="4">
         <v>23</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>123</v>
       </c>
       <c r="E25" s="3"/>
@@ -2650,10 +2647,10 @@
       <c r="B26" s="4">
         <v>24</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>125</v>
       </c>
       <c r="E26" s="3"/>
@@ -2708,10 +2705,10 @@
       <c r="B27" s="4">
         <v>25</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="11" t="s">
         <v>127</v>
       </c>
       <c r="E27" s="3"/>
@@ -2766,10 +2763,10 @@
       <c r="B28" s="4">
         <v>26</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="11" t="s">
         <v>129</v>
       </c>
       <c r="E28" s="3"/>
@@ -2824,10 +2821,10 @@
       <c r="B29" s="4">
         <v>27</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="11" t="s">
         <v>131</v>
       </c>
       <c r="E29" s="3"/>
@@ -2882,10 +2879,10 @@
       <c r="B30" s="4">
         <v>28</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E30" s="3"/>
@@ -2958,10 +2955,10 @@
       <c r="B31" s="4">
         <v>29</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="12" t="s">
         <v>135</v>
       </c>
       <c r="E31" s="3"/>
@@ -3052,8 +3049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B151" sqref="B151"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="D177" sqref="D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3089,14 +3086,16 @@
       <c r="C3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
+        <v>18792743.25</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="str">
@@ -3130,7 +3129,9 @@
       <c r="H5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="5"/>
+      <c r="I5" s="5">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="str">
@@ -3157,14 +3158,14 @@
       <c r="C7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="str">
@@ -3175,7 +3176,9 @@
         <v>45</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5">
+        <v>111011837.4825</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="2" t="s">
@@ -3215,7 +3218,9 @@
       <c r="H11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="5">
+        <v>9544.75</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="str">
@@ -3225,14 +3230,14 @@
       <c r="C12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="str">
@@ -3266,7 +3271,9 @@
       <c r="H15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="str">
@@ -3293,14 +3300,16 @@
       <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="5">
+        <v>9490.51</v>
+      </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="str">
@@ -3351,7 +3360,9 @@
       <c r="H21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I21" s="5"/>
+      <c r="I21" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="str">
@@ -3361,14 +3372,14 @@
       <c r="C22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
       <c r="H22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I22" s="7"/>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="str">
@@ -3385,7 +3396,9 @@
       <c r="H23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I23" s="5"/>
+      <c r="I23" s="5">
+        <v>46432.2</v>
+      </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="str">
@@ -3429,14 +3442,16 @@
       <c r="C27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5">
+        <v>8566623.1699999999</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
       <c r="H27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I27" s="7"/>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="str">
@@ -3470,7 +3485,9 @@
       <c r="H29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I29" s="5"/>
+      <c r="I29" s="5">
+        <v>8207.15</v>
+      </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="str">
@@ -3497,14 +3514,14 @@
       <c r="C31" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
       <c r="H31" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I31" s="7"/>
+      <c r="I31" s="5"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="str">
@@ -3515,7 +3532,9 @@
         <v>45</v>
       </c>
       <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="E33" s="5">
+        <v>1350575.4651999997</v>
+      </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="2" t="s">
@@ -3555,7 +3574,9 @@
       <c r="H35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I35" s="5"/>
+      <c r="I35" s="5">
+        <v>8258.3799999999992</v>
+      </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="str">
@@ -3565,14 +3586,14 @@
       <c r="C36" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
       <c r="H36" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I36" s="7"/>
+      <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="str">
@@ -3600,7 +3621,9 @@
         <v>45</v>
       </c>
       <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+      <c r="E39" s="5">
+        <v>178656962.39070001</v>
+      </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="2" t="s">
@@ -3633,14 +3656,16 @@
       <c r="C41" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
       <c r="H41" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I41" s="7"/>
+      <c r="I41" s="5">
+        <v>5801.89</v>
+      </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="str">
@@ -3684,7 +3709,9 @@
       <c r="C45" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="5"/>
+      <c r="D45" s="5">
+        <v>41512361</v>
+      </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
@@ -3701,14 +3728,14 @@
       <c r="C46" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
       <c r="H46" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I46" s="7"/>
+      <c r="I46" s="5"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="str">
@@ -3725,7 +3752,10 @@
       <c r="H47" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I47" s="5"/>
+      <c r="I47" s="5">
+        <f>2807*0.87*2</f>
+        <v>4884.18</v>
+      </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="str">
@@ -3769,14 +3799,16 @@
       <c r="C51" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
+      <c r="D51" s="5">
+        <v>4191975.5999999996</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
       <c r="H51" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I51" s="7"/>
+      <c r="I51" s="5"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="str">
@@ -3810,7 +3842,10 @@
       <c r="H53" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I53" s="5"/>
+      <c r="I53" s="5">
+        <f>31027*0.93</f>
+        <v>28855.11</v>
+      </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="str">
@@ -3837,14 +3872,14 @@
       <c r="C55" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
       <c r="H55" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I55" s="7"/>
+      <c r="I55" s="5"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="str">
@@ -3854,7 +3889,9 @@
       <c r="C57" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D57" s="5"/>
+      <c r="D57" s="5">
+        <v>4742988</v>
+      </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
@@ -3895,7 +3932,10 @@
       <c r="H59" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I59" s="5"/>
+      <c r="I59" s="5">
+        <f>35105*0.89</f>
+        <v>31243.45</v>
+      </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="str">
@@ -3905,14 +3945,14 @@
       <c r="C60" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
       <c r="H60" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I60" s="7"/>
+      <c r="I60" s="5"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="str">
@@ -3946,7 +3986,9 @@
       <c r="H63" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I63" s="5"/>
+      <c r="I63" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" s="4" t="str">
@@ -3973,14 +4015,16 @@
       <c r="C65" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
-      <c r="G65" s="7"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
       <c r="H65" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I65" s="7"/>
+      <c r="I65" s="5">
+        <v>37418.348023999999</v>
+      </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" s="4" t="str">
@@ -4031,7 +4075,9 @@
       <c r="H69" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I69" s="5"/>
+      <c r="I69" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="str">
@@ -4041,14 +4087,14 @@
       <c r="C70" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
       <c r="H70" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I70" s="7"/>
+      <c r="I70" s="5"/>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" s="4" t="str">
@@ -4065,7 +4111,9 @@
       <c r="H71" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I71" s="5"/>
+      <c r="I71" s="5">
+        <v>35898.094486567999</v>
+      </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="str">
@@ -4109,14 +4157,16 @@
       <c r="C75" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
       <c r="H75" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I75" s="7"/>
+      <c r="I75" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" s="4" t="str">
@@ -4150,7 +4200,9 @@
       <c r="H77" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I77" s="5"/>
+      <c r="I77" s="5">
+        <v>42580.285368026904</v>
+      </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="4" t="str">
@@ -4177,14 +4229,14 @@
       <c r="C79" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
-      <c r="G79" s="7"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
       <c r="H79" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I79" s="7"/>
+      <c r="I79" s="5"/>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B81" s="4" t="str">
@@ -4194,7 +4246,9 @@
       <c r="C81" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D81" s="5"/>
+      <c r="D81" s="5">
+        <v>812307.84</v>
+      </c>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
@@ -4235,7 +4289,10 @@
       <c r="H83" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I83" s="5"/>
+      <c r="I83" s="5">
+        <f>97175*1.2</f>
+        <v>116610</v>
+      </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" s="4" t="str">
@@ -4245,14 +4302,14 @@
       <c r="C84" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D84" s="7"/>
-      <c r="E84" s="7"/>
-      <c r="F84" s="7"/>
-      <c r="G84" s="7"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
       <c r="H84" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I84" s="7"/>
+      <c r="I84" s="5"/>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B85" s="4" t="str">
@@ -4286,7 +4343,9 @@
       <c r="H87" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I87" s="5"/>
+      <c r="I87" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B88" s="4" t="str">
@@ -4313,14 +4372,16 @@
       <c r="C89" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D89" s="7"/>
-      <c r="E89" s="7"/>
-      <c r="F89" s="7"/>
-      <c r="G89" s="7"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
       <c r="H89" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I89" s="7"/>
+      <c r="I89" s="5">
+        <v>129289</v>
+      </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B90" s="4" t="str">
@@ -4364,7 +4425,9 @@
       <c r="C93" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D93" s="5"/>
+      <c r="D93" s="5">
+        <v>90533507</v>
+      </c>
       <c r="E93" s="5"/>
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
@@ -4381,14 +4444,14 @@
       <c r="C94" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D94" s="7"/>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
       <c r="H94" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I94" s="7"/>
+      <c r="I94" s="5"/>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B95" s="4" t="str">
@@ -4405,7 +4468,10 @@
       <c r="H95" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I95" s="5"/>
+      <c r="I95" s="5">
+        <f>2865*1.25*2</f>
+        <v>7162.5</v>
+      </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B96" s="4" t="str">
@@ -4449,14 +4515,16 @@
       <c r="C99" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D99" s="7"/>
-      <c r="E99" s="7"/>
-      <c r="F99" s="7"/>
-      <c r="G99" s="7"/>
+      <c r="D99" s="5">
+        <v>13888870</v>
+      </c>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
       <c r="H99" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I99" s="7"/>
+      <c r="I99" s="5"/>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B100" s="4" t="str">
@@ -4490,7 +4558,10 @@
       <c r="H101" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I101" s="5"/>
+      <c r="I101" s="5">
+        <f>31056*1.07</f>
+        <v>33229.920000000006</v>
+      </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B102" s="4" t="str">
@@ -4517,14 +4588,14 @@
       <c r="C103" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D103" s="7"/>
-      <c r="E103" s="7"/>
-      <c r="F103" s="7"/>
-      <c r="G103" s="7"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
       <c r="H103" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I103" s="7"/>
+      <c r="I103" s="5"/>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B105" s="4" t="str">
@@ -4534,7 +4605,9 @@
       <c r="C105" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D105" s="5"/>
+      <c r="D105" s="5">
+        <v>15712783</v>
+      </c>
       <c r="E105" s="5"/>
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
@@ -4575,7 +4648,10 @@
       <c r="H107" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I107" s="5"/>
+      <c r="I107" s="5">
+        <f>35134*1.07</f>
+        <v>37593.380000000005</v>
+      </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B108" s="4" t="str">
@@ -4585,14 +4661,14 @@
       <c r="C108" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D108" s="7"/>
-      <c r="E108" s="7"/>
-      <c r="F108" s="7"/>
-      <c r="G108" s="7"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="5"/>
       <c r="H108" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I108" s="7"/>
+      <c r="I108" s="5"/>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B109" s="4" t="str">
@@ -4626,7 +4702,9 @@
       <c r="H111" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I111" s="5"/>
+      <c r="I111" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B112" s="4" t="str">
@@ -4653,14 +4731,16 @@
       <c r="C113" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D113" s="7"/>
-      <c r="E113" s="7"/>
-      <c r="F113" s="7"/>
-      <c r="G113" s="7"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="5"/>
+      <c r="G113" s="5"/>
       <c r="H113" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I113" s="7"/>
+      <c r="I113" s="5">
+        <v>40130</v>
+      </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B114" s="4" t="str">
@@ -4704,7 +4784,9 @@
       <c r="C117" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D117" s="5"/>
+      <c r="D117" s="5">
+        <v>2388215.0627615061</v>
+      </c>
       <c r="E117" s="5"/>
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
@@ -4721,14 +4803,14 @@
       <c r="C118" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D118" s="7"/>
-      <c r="E118" s="7"/>
-      <c r="F118" s="7"/>
-      <c r="G118" s="7"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="5"/>
+      <c r="G118" s="5"/>
       <c r="H118" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I118" s="7"/>
+      <c r="I118" s="5"/>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B119" s="4" t="str">
@@ -4745,7 +4827,9 @@
       <c r="H119" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I119" s="5"/>
+      <c r="I119" s="5">
+        <v>116644.8</v>
+      </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B120" s="4" t="str">
@@ -4789,14 +4873,16 @@
       <c r="C123" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D123" s="7"/>
-      <c r="E123" s="7"/>
-      <c r="F123" s="7"/>
-      <c r="G123" s="7"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="5"/>
+      <c r="F123" s="5"/>
+      <c r="G123" s="5"/>
       <c r="H123" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I123" s="7"/>
+      <c r="I123" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B124" s="4" t="str">
@@ -4830,7 +4916,9 @@
       <c r="H125" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I125" s="5"/>
+      <c r="I125" s="5">
+        <v>129322</v>
+      </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B126" s="4" t="str">
@@ -4857,14 +4945,14 @@
       <c r="C127" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D127" s="7"/>
-      <c r="E127" s="7"/>
-      <c r="F127" s="7"/>
-      <c r="G127" s="7"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="5"/>
+      <c r="G127" s="5"/>
       <c r="H127" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I127" s="7"/>
+      <c r="I127" s="5"/>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B129" s="4" t="str">
@@ -4881,7 +4969,9 @@
       <c r="H129" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I129" s="5"/>
+      <c r="I129" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B130" s="4" t="str">
@@ -4915,7 +5005,9 @@
       <c r="H131" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I131" s="5"/>
+      <c r="I131" s="5">
+        <v>2806.8920419999999</v>
+      </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B132" s="4" t="str">
@@ -4925,14 +5017,14 @@
       <c r="C132" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D132" s="7"/>
-      <c r="E132" s="7"/>
-      <c r="F132" s="7"/>
-      <c r="G132" s="7"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+      <c r="G132" s="5"/>
       <c r="H132" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I132" s="7"/>
+      <c r="I132" s="5"/>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B133" s="4" t="str">
@@ -4966,7 +5058,9 @@
       <c r="H135" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I135" s="5"/>
+      <c r="I135" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B136" s="4" t="str">
@@ -4993,14 +5087,16 @@
       <c r="C137" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D137" s="7"/>
-      <c r="E137" s="7"/>
-      <c r="F137" s="7"/>
-      <c r="G137" s="7"/>
+      <c r="D137" s="5"/>
+      <c r="E137" s="5"/>
+      <c r="F137" s="5"/>
+      <c r="G137" s="5"/>
       <c r="H137" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I137" s="7"/>
+      <c r="I137" s="5">
+        <v>40078.903184151503</v>
+      </c>
     </row>
     <row r="138" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B138" s="4" t="str">
@@ -5051,7 +5147,9 @@
       <c r="H141" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I141" s="5"/>
+      <c r="I141" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B142" s="4" t="str">
@@ -5061,14 +5159,14 @@
       <c r="C142" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D142" s="7"/>
-      <c r="E142" s="7"/>
-      <c r="F142" s="7"/>
-      <c r="G142" s="7"/>
+      <c r="D142" s="5"/>
+      <c r="E142" s="5"/>
+      <c r="F142" s="5"/>
+      <c r="G142" s="5"/>
       <c r="H142" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I142" s="7"/>
+      <c r="I142" s="5"/>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B143" s="4" t="str">
@@ -5085,7 +5183,9 @@
       <c r="H143" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I143" s="5"/>
+      <c r="I143" s="5">
+        <v>129288.521246736</v>
+      </c>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B144" s="4" t="str">
@@ -5129,14 +5229,16 @@
       <c r="C147" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D147" s="7"/>
-      <c r="E147" s="7"/>
-      <c r="F147" s="7"/>
-      <c r="G147" s="7"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="5"/>
+      <c r="F147" s="5"/>
+      <c r="G147" s="5"/>
       <c r="H147" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I147" s="7"/>
+      <c r="I147" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B148" s="4" t="str">
@@ -5170,7 +5272,9 @@
       <c r="H149" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I149" s="5"/>
+      <c r="I149" s="5">
+        <v>2808.488042</v>
+      </c>
     </row>
     <row r="150" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B150" s="4" t="str">
@@ -5214,14 +5318,16 @@
       <c r="C153" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D153" s="7"/>
-      <c r="E153" s="7"/>
-      <c r="F153" s="7"/>
-      <c r="G153" s="7"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="5"/>
+      <c r="F153" s="5"/>
+      <c r="G153" s="5"/>
       <c r="H153" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I153" s="7"/>
+      <c r="I153" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="154" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B154" s="4" t="str">
@@ -5255,7 +5361,9 @@
       <c r="H155" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I155" s="5"/>
+      <c r="I155" s="5">
+        <v>40109.651281712439</v>
+      </c>
     </row>
     <row r="156" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B156" s="4" t="str">
@@ -5299,14 +5407,16 @@
       <c r="C159" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D159" s="7"/>
-      <c r="E159" s="7"/>
-      <c r="F159" s="7"/>
-      <c r="G159" s="7"/>
+      <c r="D159" s="5"/>
+      <c r="E159" s="5"/>
+      <c r="F159" s="5"/>
+      <c r="G159" s="5"/>
       <c r="H159" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I159" s="7"/>
+      <c r="I159" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="160" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B160" s="4" t="str">
@@ -5340,7 +5450,9 @@
       <c r="H161" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I161" s="5"/>
+      <c r="I161" s="5">
+        <v>129288.52124673559</v>
+      </c>
     </row>
     <row r="162" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B162" s="4" t="str">
@@ -5384,14 +5496,16 @@
       <c r="C165" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D165" s="7"/>
-      <c r="E165" s="7"/>
-      <c r="F165" s="7"/>
-      <c r="G165" s="7"/>
+      <c r="D165" s="5"/>
+      <c r="E165" s="5">
+        <v>9020990.7095999997</v>
+      </c>
+      <c r="F165" s="5"/>
+      <c r="G165" s="5"/>
       <c r="H165" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I165" s="7"/>
+      <c r="I165" s="5"/>
     </row>
     <row r="166" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B166" s="4" t="str">
@@ -5425,7 +5539,9 @@
       <c r="H167" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I167" s="5"/>
+      <c r="I167" s="5">
+        <v>915</v>
+      </c>
     </row>
     <row r="168" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B168" s="4" t="str">
@@ -5469,14 +5585,16 @@
       <c r="C171" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D171" s="7"/>
-      <c r="E171" s="7"/>
-      <c r="F171" s="7"/>
-      <c r="G171" s="7"/>
+      <c r="D171" s="5"/>
+      <c r="E171" s="5">
+        <v>7956362.0040000016</v>
+      </c>
+      <c r="F171" s="5"/>
+      <c r="G171" s="5"/>
       <c r="H171" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I171" s="7"/>
+      <c r="I171" s="5"/>
     </row>
     <row r="172" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B172" s="4" t="str">
@@ -5510,7 +5628,9 @@
       <c r="H173" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I173" s="5"/>
+      <c r="I173" s="5">
+        <v>915</v>
+      </c>
     </row>
     <row r="174" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B174" s="4" t="str">
@@ -5548,6 +5668,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5569,7 +5690,7 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix outputting uncertainty cells
</commit_message>
<xml_diff>
--- a/tests/databooks/progbook_tb.xlsx
+++ b/tests/databooks/progbook_tb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD43AF1-0508-4C08-B029-E4ABB85CD0BC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B75AFB-269B-4E28-9F49-E78165B63790}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="26160" windowHeight="15195" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="26160" windowHeight="15195" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program targeting" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="138">
   <si>
     <t>Targeted to (populations)</t>
   </si>
@@ -949,7 +949,8 @@
   <dimension ref="A1:AO31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AO3" sqref="N3:AO33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2422,8 +2423,12 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
+      <c r="I24" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="K24" s="4"/>
       <c r="L24" s="10"/>
       <c r="N24" s="7"/>
@@ -2472,8 +2477,12 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="I25" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="K25" s="4"/>
       <c r="L25" s="10"/>
       <c r="N25" s="7"/>
@@ -2522,8 +2531,12 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
+      <c r="I26" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="K26" s="4"/>
       <c r="L26" s="10"/>
       <c r="N26" s="7"/>
@@ -2574,8 +2587,12 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="10"/>
+      <c r="K27" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="L27" s="10" t="s">
+        <v>132</v>
+      </c>
       <c r="N27" s="7"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
@@ -2624,8 +2641,12 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="10"/>
+      <c r="K28" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>132</v>
+      </c>
       <c r="N28" s="7"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
@@ -2674,8 +2695,12 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="10"/>
+      <c r="K29" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="L29" s="10" t="s">
+        <v>132</v>
+      </c>
       <c r="N29" s="7"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
@@ -2852,8 +2877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H173"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="G31:H35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2891,7 +2916,9 @@
       <c r="A2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="11">
+        <v>50</v>
+      </c>
       <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
         <v>42</v>
@@ -2907,7 +2934,9 @@
       <c r="A3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="11">
+        <v>5</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1" t="s">
         <v>42</v>
@@ -2921,7 +2950,9 @@
       <c r="A4" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="11">
+        <v>0</v>
+      </c>
       <c r="C4" s="4">
         <v>56</v>
       </c>
@@ -2937,7 +2968,9 @@
       <c r="A5" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="1" t="s">
         <v>42</v>
@@ -2993,7 +3026,9 @@
       <c r="A9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="11">
+        <v>50</v>
+      </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
         <v>42</v>
@@ -3093,7 +3128,9 @@
       <c r="A16" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="11">
+        <v>50</v>
+      </c>
       <c r="C16" s="4">
         <v>9490.51</v>
       </c>
@@ -5374,8 +5411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U14" sqref="G14:U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>